<commit_message>
galadhrim guard upgrade fix
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57215DF-66B4-44BB-94DC-0BFA34AFA88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F857BB-59C7-4FFC-AA2D-F0470359BB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5771" uniqueCount="1634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1635">
   <si>
     <t>faction</t>
   </si>
@@ -5077,6 +5077,9 @@
   </si>
   <si>
     <t>["[sharkey's_rogues] hobbit_militia"]</t>
+  </si>
+  <si>
+    <t>['Galadhrim Guard Upgrade']</t>
   </si>
 </sst>
 </file>
@@ -5531,23 +5534,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
   <dimension ref="A1:J392"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A374" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A392" sqref="A392"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18501,17 +18504,17 @@
   <dimension ref="A1:H633"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A523" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C536" sqref="C536"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D145" sqref="D145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -21997,6 +22000,9 @@
       </c>
       <c r="E145">
         <v>1</v>
+      </c>
+      <c r="F145" t="s">
+        <v>402</v>
       </c>
       <c r="G145">
         <v>0</v>
@@ -33798,12 +33804,12 @@
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" customWidth="1"/>
+    <col min="4" max="4" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -33820,7 +33826,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60">
+    <row r="2" spans="1:4" ht="57.6">
       <c r="A2" s="6" t="s">
         <v>132</v>
       </c>
@@ -33834,7 +33840,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="43.2">
       <c r="A3" s="6" t="s">
         <v>95</v>
       </c>
@@ -33848,7 +33854,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="135">
+    <row r="4" spans="1:4" ht="115.2">
       <c r="A4" s="6" t="s">
         <v>124</v>
       </c>
@@ -33862,7 +33868,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105">
+    <row r="5" spans="1:4" ht="100.8">
       <c r="A5" s="6" t="s">
         <v>846</v>
       </c>
@@ -33872,7 +33878,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" ht="90">
+    <row r="6" spans="1:4" ht="72">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -33886,7 +33892,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="75">
+    <row r="7" spans="1:4" ht="72">
       <c r="A7" s="6" t="s">
         <v>851</v>
       </c>
@@ -33900,7 +33906,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60">
+    <row r="8" spans="1:4" ht="57.6">
       <c r="A8" s="6" t="s">
         <v>71</v>
       </c>
@@ -33914,7 +33920,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="45">
+    <row r="9" spans="1:4" ht="28.8">
       <c r="A9" s="6" t="s">
         <v>858</v>
       </c>
@@ -33928,7 +33934,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="180">
+    <row r="10" spans="1:4" ht="144">
       <c r="A10" s="6" t="s">
         <v>862</v>
       </c>
@@ -33938,7 +33944,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" ht="120">
+    <row r="11" spans="1:4" ht="115.2">
       <c r="A11" s="6" t="s">
         <v>864</v>
       </c>
@@ -33948,7 +33954,7 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" ht="45">
+    <row r="12" spans="1:4" ht="43.2">
       <c r="A12" s="6" t="s">
         <v>241</v>
       </c>
@@ -33962,7 +33968,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="90">
+    <row r="13" spans="1:4" ht="86.4">
       <c r="A13" s="6" t="s">
         <v>869</v>
       </c>
@@ -33976,7 +33982,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="75">
+    <row r="14" spans="1:4" ht="57.6">
       <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
@@ -33990,7 +33996,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="255">
+    <row r="15" spans="1:4" ht="244.8">
       <c r="A15" s="6" t="s">
         <v>875</v>
       </c>
@@ -34000,7 +34006,7 @@
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="285">
+    <row r="16" spans="1:4" ht="273.60000000000002">
       <c r="A16" s="6" t="s">
         <v>877</v>
       </c>
@@ -34010,7 +34016,7 @@
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
     </row>
-    <row r="17" spans="1:4" ht="405">
+    <row r="17" spans="1:4" ht="360">
       <c r="A17" s="6" t="s">
         <v>879</v>
       </c>
@@ -34020,7 +34026,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="45">
+    <row r="18" spans="1:4" ht="43.2">
       <c r="A18" s="6" t="s">
         <v>881</v>
       </c>
@@ -34034,7 +34040,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="105">
+    <row r="19" spans="1:4" ht="100.8">
       <c r="A19" s="6" t="s">
         <v>885</v>
       </c>
@@ -34044,7 +34050,7 @@
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="105">
+    <row r="20" spans="1:4" ht="100.8">
       <c r="A20" s="6" t="s">
         <v>887</v>
       </c>
@@ -34054,7 +34060,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="75">
+    <row r="21" spans="1:4" ht="72">
       <c r="A21" s="6" t="s">
         <v>242</v>
       </c>
@@ -34068,7 +34074,7 @@
         <v>891</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="135">
+    <row r="22" spans="1:4" ht="129.6">
       <c r="A22" s="6" t="s">
         <v>245</v>
       </c>
@@ -34078,7 +34084,7 @@
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" ht="90">
+    <row r="23" spans="1:4" ht="72">
       <c r="A23" s="6" t="s">
         <v>239</v>
       </c>
@@ -34092,7 +34098,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30">
+    <row r="24" spans="1:4" ht="28.8">
       <c r="A24" s="6" t="s">
         <v>895</v>
       </c>
@@ -34106,7 +34112,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45">
+    <row r="25" spans="1:4" ht="43.2">
       <c r="A25" s="6" t="s">
         <v>899</v>
       </c>
@@ -34120,7 +34126,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="409.5">
+    <row r="26" spans="1:4" ht="409.6">
       <c r="A26" s="6" t="s">
         <v>903</v>
       </c>
@@ -34130,7 +34136,7 @@
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
     </row>
-    <row r="27" spans="1:4" ht="165">
+    <row r="27" spans="1:4" ht="158.4">
       <c r="A27" s="6" t="s">
         <v>905</v>
       </c>
@@ -34140,7 +34146,7 @@
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="255">
+    <row r="28" spans="1:4" ht="230.4">
       <c r="A28" s="6" t="s">
         <v>907</v>
       </c>
@@ -34150,7 +34156,7 @@
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" ht="60">
+    <row r="29" spans="1:4" ht="43.2">
       <c r="A29" s="6" t="s">
         <v>909</v>
       </c>
@@ -34164,7 +34170,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="45">
+    <row r="30" spans="1:4" ht="43.2">
       <c r="A30" s="6" t="s">
         <v>243</v>
       </c>
@@ -34176,7 +34182,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45">
+    <row r="31" spans="1:4" ht="43.2">
       <c r="A31" s="6" t="s">
         <v>246</v>
       </c>
@@ -34187,7 +34193,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="120">
+    <row r="32" spans="1:4" ht="100.8">
       <c r="A32" s="6" t="s">
         <v>206</v>
       </c>
@@ -34201,7 +34207,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="180">
+    <row r="33" spans="1:4" ht="172.8">
       <c r="A33" s="6" t="s">
         <v>244</v>
       </c>
@@ -34211,7 +34217,7 @@
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="30">
+    <row r="34" spans="1:4" ht="28.8">
       <c r="A34" s="6" t="s">
         <v>917</v>
       </c>
@@ -34225,7 +34231,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="120">
+    <row r="35" spans="1:4" ht="100.8">
       <c r="A35" s="6" t="s">
         <v>921</v>
       </c>
@@ -34239,7 +34245,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="375">
+    <row r="36" spans="1:4" ht="331.2">
       <c r="A36" s="6" t="s">
         <v>923</v>
       </c>
@@ -34249,7 +34255,7 @@
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
     </row>
-    <row r="37" spans="1:4" ht="75">
+    <row r="37" spans="1:4" ht="72">
       <c r="A37" s="6" t="s">
         <v>925</v>
       </c>
@@ -34263,7 +34269,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45">
+    <row r="38" spans="1:4" ht="43.2">
       <c r="A38" s="6" t="s">
         <v>929</v>
       </c>
@@ -34277,7 +34283,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="75">
+    <row r="39" spans="1:4" ht="72">
       <c r="A39" s="6" t="s">
         <v>933</v>
       </c>
@@ -34287,7 +34293,7 @@
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
     </row>
-    <row r="40" spans="1:4" ht="300">
+    <row r="40" spans="1:4" ht="244.8">
       <c r="A40" s="6" t="s">
         <v>935</v>
       </c>
@@ -34297,7 +34303,7 @@
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
     </row>
-    <row r="41" spans="1:4" ht="135">
+    <row r="41" spans="1:4" ht="115.2">
       <c r="A41" s="6" t="s">
         <v>937</v>
       </c>
@@ -34307,7 +34313,7 @@
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
     </row>
-    <row r="42" spans="1:4" ht="45">
+    <row r="42" spans="1:4" ht="43.2">
       <c r="A42" s="6" t="s">
         <v>939</v>
       </c>
@@ -34321,7 +34327,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="120">
+    <row r="43" spans="1:4" ht="115.2">
       <c r="A43" s="6" t="s">
         <v>943</v>
       </c>
@@ -34331,7 +34337,7 @@
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
     </row>
-    <row r="44" spans="1:4" ht="135">
+    <row r="44" spans="1:4" ht="129.6">
       <c r="A44" s="6" t="s">
         <v>58</v>
       </c>
@@ -34345,7 +34351,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="150">
+    <row r="45" spans="1:4" ht="129.6">
       <c r="A45" s="6" t="s">
         <v>948</v>
       </c>
@@ -34359,7 +34365,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="60">
+    <row r="46" spans="1:4" ht="43.2">
       <c r="A46" s="6" t="s">
         <v>951</v>
       </c>
@@ -34373,7 +34379,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60">
+    <row r="47" spans="1:4" ht="57.6">
       <c r="A47" s="6" t="s">
         <v>955</v>
       </c>
@@ -34387,7 +34393,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="135">
+    <row r="48" spans="1:4" ht="115.2">
       <c r="A48" s="6" t="s">
         <v>208</v>
       </c>
@@ -34401,7 +34407,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="45">
+    <row r="49" spans="1:4" ht="43.2">
       <c r="A49" s="6" t="s">
         <v>962</v>
       </c>
@@ -34415,7 +34421,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="90">
+    <row r="50" spans="1:4" ht="86.4">
       <c r="A50" s="6" t="s">
         <v>965</v>
       </c>
@@ -34429,7 +34435,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="75">
+    <row r="51" spans="1:4" ht="57.6">
       <c r="A51" s="6" t="s">
         <v>207</v>
       </c>
@@ -34443,7 +34449,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="210">
+    <row r="52" spans="1:4" ht="201.6">
       <c r="A52" s="6" t="s">
         <v>971</v>
       </c>
@@ -34453,7 +34459,7 @@
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
     </row>
-    <row r="53" spans="1:4" ht="405">
+    <row r="53" spans="1:4" ht="360">
       <c r="A53" s="6" t="s">
         <v>973</v>
       </c>
@@ -34463,7 +34469,7 @@
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
     </row>
-    <row r="54" spans="1:4" ht="75">
+    <row r="54" spans="1:4" ht="72">
       <c r="A54" s="6" t="s">
         <v>975</v>
       </c>
@@ -34477,7 +34483,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="135">
+    <row r="55" spans="1:4" ht="115.2">
       <c r="A55" s="6" t="s">
         <v>979</v>
       </c>
@@ -34491,7 +34497,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="300">
+    <row r="56" spans="1:4" ht="259.2">
       <c r="A56" s="6" t="s">
         <v>982</v>
       </c>
@@ -34501,7 +34507,7 @@
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
     </row>
-    <row r="57" spans="1:4" ht="135">
+    <row r="57" spans="1:4" ht="115.2">
       <c r="A57" s="6" t="s">
         <v>984</v>
       </c>
@@ -34515,7 +34521,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="315">
+    <row r="58" spans="1:4" ht="288">
       <c r="A58" s="6" t="s">
         <v>987</v>
       </c>
@@ -34525,7 +34531,7 @@
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4" ht="255">
+    <row r="59" spans="1:4" ht="216">
       <c r="A59" s="6" t="s">
         <v>989</v>
       </c>
@@ -34535,7 +34541,7 @@
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
     </row>
-    <row r="60" spans="1:4" ht="45">
+    <row r="60" spans="1:4" ht="43.2">
       <c r="A60" s="6" t="s">
         <v>209</v>
       </c>
@@ -34549,7 +34555,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30">
+    <row r="61" spans="1:4" ht="28.8">
       <c r="A61" s="6" t="s">
         <v>994</v>
       </c>
@@ -34563,7 +34569,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="409.5">
+    <row r="62" spans="1:4" ht="409.6">
       <c r="A62" s="6" t="s">
         <v>998</v>
       </c>
@@ -34573,7 +34579,7 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
     </row>
-    <row r="63" spans="1:4" ht="409.5">
+    <row r="63" spans="1:4" ht="409.6">
       <c r="A63" s="6" t="s">
         <v>1000</v>
       </c>
@@ -34583,7 +34589,7 @@
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="1:4" ht="45">
+    <row r="64" spans="1:4" ht="43.2">
       <c r="A64" s="6" t="s">
         <v>1002</v>
       </c>
@@ -34597,7 +34603,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45">
+    <row r="65" spans="1:4" ht="43.2">
       <c r="A65" s="6" t="s">
         <v>1005</v>
       </c>
@@ -34611,7 +34617,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="165">
+    <row r="66" spans="1:4" ht="158.4">
       <c r="A66" s="6" t="s">
         <v>1009</v>
       </c>
@@ -34621,7 +34627,7 @@
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
     </row>
-    <row r="67" spans="1:4" ht="45">
+    <row r="67" spans="1:4" ht="43.2">
       <c r="A67" s="6" t="s">
         <v>1011</v>
       </c>
@@ -34635,7 +34641,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="409.5">
+    <row r="68" spans="1:4" ht="403.2">
       <c r="A68" s="6" t="s">
         <v>1014</v>
       </c>
@@ -34645,7 +34651,7 @@
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
     </row>
-    <row r="69" spans="1:4" ht="75">
+    <row r="69" spans="1:4" ht="72">
       <c r="A69" s="6" t="s">
         <v>1016</v>
       </c>
@@ -34659,7 +34665,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="210">
+    <row r="70" spans="1:4" ht="187.2">
       <c r="A70" s="6" t="s">
         <v>1019</v>
       </c>
@@ -34669,7 +34675,7 @@
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
     </row>
-    <row r="71" spans="1:4" ht="270">
+    <row r="71" spans="1:4" ht="244.8">
       <c r="A71" s="6" t="s">
         <v>1021</v>
       </c>
@@ -34679,7 +34685,7 @@
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="1:4" ht="390">
+    <row r="72" spans="1:4" ht="374.4">
       <c r="A72" s="6" t="s">
         <v>1023</v>
       </c>
@@ -34689,7 +34695,7 @@
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
     </row>
-    <row r="73" spans="1:4" ht="105">
+    <row r="73" spans="1:4" ht="100.8">
       <c r="A73" s="6" t="s">
         <v>1025</v>
       </c>
@@ -34703,7 +34709,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="105">
+    <row r="74" spans="1:4" ht="100.8">
       <c r="A74" s="6" t="s">
         <v>1028</v>
       </c>
@@ -34713,7 +34719,7 @@
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
     </row>
-    <row r="75" spans="1:4" ht="60">
+    <row r="75" spans="1:4" ht="43.2">
       <c r="A75" s="6" t="s">
         <v>1030</v>
       </c>
@@ -34727,7 +34733,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="150">
+    <row r="76" spans="1:4" ht="144">
       <c r="A76" s="6" t="s">
         <v>1033</v>
       </c>
@@ -34737,7 +34743,7 @@
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
     </row>
-    <row r="77" spans="1:4" ht="90">
+    <row r="77" spans="1:4" ht="72">
       <c r="A77" s="6" t="s">
         <v>1035</v>
       </c>
@@ -34751,7 +34757,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="165">
+    <row r="78" spans="1:4" ht="158.4">
       <c r="A78" s="6" t="s">
         <v>1037</v>
       </c>
@@ -34761,7 +34767,7 @@
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
     </row>
-    <row r="79" spans="1:4" ht="390">
+    <row r="79" spans="1:4" ht="360">
       <c r="A79" s="6" t="s">
         <v>1039</v>
       </c>
@@ -34771,7 +34777,7 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="1:4" ht="30">
+    <row r="80" spans="1:4" ht="28.8">
       <c r="A80" s="6" t="s">
         <v>1041</v>
       </c>
@@ -34790,16 +34796,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="62" customWidth="1"/>
-    <col min="2" max="2" width="111.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="111.88671875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -34813,7 +34819,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30">
+    <row r="2" spans="1:3" ht="28.8">
       <c r="A2" s="9" t="s">
         <v>1287</v>
       </c>
@@ -34824,7 +34830,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="28.8">
       <c r="A3" s="9" t="s">
         <v>1288</v>
       </c>
@@ -34835,7 +34841,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="28.8">
       <c r="A4" s="9" t="s">
         <v>1289</v>
       </c>
@@ -34846,7 +34852,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" s="9" t="s">
         <v>1061</v>
       </c>
@@ -34857,7 +34863,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="28.8">
       <c r="A6" s="9" t="s">
         <v>1290</v>
       </c>
@@ -34868,7 +34874,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="28.8">
       <c r="A7" s="9" t="s">
         <v>1062</v>
       </c>
@@ -34879,7 +34885,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="28.8">
       <c r="A8" s="9" t="s">
         <v>1063</v>
       </c>
@@ -34890,7 +34896,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30">
+    <row r="9" spans="1:3" ht="28.8">
       <c r="A9" s="9" t="s">
         <v>1291</v>
       </c>
@@ -34901,7 +34907,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
+    <row r="10" spans="1:3" ht="28.8">
       <c r="A10" s="9" t="s">
         <v>1292</v>
       </c>
@@ -34912,7 +34918,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30">
+    <row r="11" spans="1:3" ht="28.8">
       <c r="A11" s="9" t="s">
         <v>1063</v>
       </c>
@@ -34923,7 +34929,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30">
+    <row r="12" spans="1:3" ht="28.8">
       <c r="A12" s="14" t="s">
         <v>1310</v>
       </c>
@@ -34934,7 +34940,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30">
+    <row r="13" spans="1:3" ht="28.8">
       <c r="A13" s="14" t="s">
         <v>1311</v>
       </c>
@@ -34945,7 +34951,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3" ht="28.8">
       <c r="A14" s="9" t="s">
         <v>1051</v>
       </c>
@@ -34956,7 +34962,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="28.8">
       <c r="A15" s="9" t="s">
         <v>1052</v>
       </c>
@@ -34967,7 +34973,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="9" t="s">
         <v>1053</v>
       </c>
@@ -34978,7 +34984,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" s="9" t="s">
         <v>1054</v>
       </c>
@@ -34989,7 +34995,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="28.8">
       <c r="A18" s="9" t="s">
         <v>1055</v>
       </c>
@@ -35000,7 +35006,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30">
+    <row r="19" spans="1:3" ht="28.8">
       <c r="A19" s="9" t="s">
         <v>1056</v>
       </c>
@@ -35011,7 +35017,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30">
+    <row r="20" spans="1:3" ht="28.8">
       <c r="A20" s="9" t="s">
         <v>1057</v>
       </c>
@@ -35044,7 +35050,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30">
+    <row r="23" spans="1:3" ht="28.8">
       <c r="A23" s="9" t="s">
         <v>1060</v>
       </c>
@@ -35066,7 +35072,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="60">
+    <row r="25" spans="1:3" ht="57.6">
       <c r="A25" s="12" t="s">
         <v>1065</v>
       </c>
@@ -35077,7 +35083,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="60">
+    <row r="26" spans="1:3" ht="57.6">
       <c r="A26" s="12" t="s">
         <v>1066</v>
       </c>
@@ -35088,7 +35094,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60">
+    <row r="27" spans="1:3" ht="57.6">
       <c r="A27" s="12" t="s">
         <v>1067</v>
       </c>
@@ -35099,7 +35105,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="60">
+    <row r="28" spans="1:3" ht="57.6">
       <c r="A28" s="12" t="s">
         <v>1068</v>
       </c>
@@ -35110,7 +35116,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="60">
+    <row r="29" spans="1:3" ht="57.6">
       <c r="A29" s="12" t="s">
         <v>1069</v>
       </c>
@@ -35121,7 +35127,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="60">
+    <row r="30" spans="1:3" ht="57.6">
       <c r="A30" s="12" t="s">
         <v>1070</v>
       </c>
@@ -35132,7 +35138,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="60">
+    <row r="31" spans="1:3" ht="57.6">
       <c r="A31" s="12" t="s">
         <v>1071</v>
       </c>
@@ -35143,7 +35149,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="60">
+    <row r="32" spans="1:3" ht="57.6">
       <c r="A32" s="12" t="s">
         <v>1072</v>
       </c>
@@ -35154,7 +35160,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="60">
+    <row r="33" spans="1:3" ht="57.6">
       <c r="A33" s="12" t="s">
         <v>1073</v>
       </c>
@@ -35165,7 +35171,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60">
+    <row r="34" spans="1:3" ht="57.6">
       <c r="A34" s="12" t="s">
         <v>1074</v>
       </c>
@@ -35176,7 +35182,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="60">
+    <row r="35" spans="1:3" ht="57.6">
       <c r="A35" s="12" t="s">
         <v>1075</v>
       </c>
@@ -35187,7 +35193,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="60">
+    <row r="36" spans="1:3" ht="57.6">
       <c r="A36" s="12" t="s">
         <v>1076</v>
       </c>
@@ -35198,7 +35204,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="60">
+    <row r="37" spans="1:3" ht="57.6">
       <c r="A37" s="12" t="s">
         <v>1077</v>
       </c>
@@ -35209,7 +35215,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="60">
+    <row r="38" spans="1:3" ht="57.6">
       <c r="A38" s="12" t="s">
         <v>1078</v>
       </c>
@@ -35220,7 +35226,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="60">
+    <row r="39" spans="1:3" ht="57.6">
       <c r="A39" s="12" t="s">
         <v>1079</v>
       </c>
@@ -35253,7 +35259,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="60">
+    <row r="42" spans="1:3" ht="57.6">
       <c r="A42" s="12" t="s">
         <v>1082</v>
       </c>
@@ -35264,7 +35270,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30">
+    <row r="43" spans="1:3" ht="28.8">
       <c r="A43" s="9" t="s">
         <v>1084</v>
       </c>
@@ -35275,7 +35281,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30">
+    <row r="44" spans="1:3" ht="28.8">
       <c r="A44" s="9" t="s">
         <v>1085</v>
       </c>
@@ -35286,7 +35292,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30">
+    <row r="45" spans="1:3" ht="28.8">
       <c r="A45" s="9" t="s">
         <v>1086</v>
       </c>
@@ -35297,7 +35303,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30">
+    <row r="46" spans="1:3" ht="28.8">
       <c r="A46" s="9" t="s">
         <v>1087</v>
       </c>
@@ -35308,7 +35314,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="30">
+    <row r="47" spans="1:3" ht="28.8">
       <c r="A47" s="9" t="s">
         <v>1088</v>
       </c>
@@ -35319,7 +35325,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="30">
+    <row r="48" spans="1:3" ht="28.8">
       <c r="A48" s="9" t="s">
         <v>1089</v>
       </c>
@@ -35327,10 +35333,10 @@
         <v>1092</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="30">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="28.8">
       <c r="A49" s="9" t="s">
         <v>1090</v>
       </c>
@@ -35338,10 +35344,10 @@
         <v>1092</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="30">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="28.8">
       <c r="A50" s="9" t="s">
         <v>1091</v>
       </c>
@@ -35352,7 +35358,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="45">
+    <row r="51" spans="1:3" ht="28.8">
       <c r="A51" s="12" t="s">
         <v>1093</v>
       </c>
@@ -35363,7 +35369,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="45">
+    <row r="52" spans="1:3" ht="28.8">
       <c r="A52" s="12" t="s">
         <v>1094</v>
       </c>
@@ -35374,7 +35380,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="45">
+    <row r="53" spans="1:3" ht="28.8">
       <c r="A53" s="12" t="s">
         <v>1095</v>
       </c>
@@ -35385,7 +35391,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="45">
+    <row r="54" spans="1:3" ht="28.8">
       <c r="A54" s="12" t="s">
         <v>1096</v>
       </c>
@@ -35396,7 +35402,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="45">
+    <row r="55" spans="1:3" ht="28.8">
       <c r="A55" s="12" t="s">
         <v>1097</v>
       </c>
@@ -35407,7 +35413,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="45">
+    <row r="56" spans="1:3" ht="28.8">
       <c r="A56" s="12" t="s">
         <v>1098</v>
       </c>
@@ -35418,7 +35424,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="45">
+    <row r="57" spans="1:3" ht="28.8">
       <c r="A57" s="12" t="s">
         <v>1099</v>
       </c>
@@ -35429,7 +35435,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="45">
+    <row r="58" spans="1:3" ht="28.8">
       <c r="A58" s="12" t="s">
         <v>1100</v>
       </c>
@@ -35440,7 +35446,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="45">
+    <row r="59" spans="1:3" ht="28.8">
       <c r="A59" s="12" t="s">
         <v>1101</v>
       </c>
@@ -35451,7 +35457,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="45">
+    <row r="60" spans="1:3" ht="28.8">
       <c r="A60" s="12" t="s">
         <v>1102</v>
       </c>
@@ -35462,7 +35468,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="45">
+    <row r="61" spans="1:3" ht="28.8">
       <c r="A61" s="12" t="s">
         <v>1103</v>
       </c>
@@ -35473,7 +35479,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="45">
+    <row r="62" spans="1:3" ht="28.8">
       <c r="A62" s="12" t="s">
         <v>1104</v>
       </c>
@@ -35484,7 +35490,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="45">
+    <row r="63" spans="1:3" ht="28.8">
       <c r="A63" s="12" t="s">
         <v>1105</v>
       </c>
@@ -35506,7 +35512,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="45">
+    <row r="65" spans="1:3" ht="28.8">
       <c r="A65" s="12" t="s">
         <v>1106</v>
       </c>
@@ -35517,7 +35523,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="45">
+    <row r="66" spans="1:3" ht="28.8">
       <c r="A66" s="12" t="s">
         <v>1107</v>
       </c>
@@ -35528,7 +35534,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="45">
+    <row r="67" spans="1:3" ht="28.8">
       <c r="A67" s="12" t="s">
         <v>1108</v>
       </c>
@@ -35539,7 +35545,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="45">
+    <row r="68" spans="1:3" ht="28.8">
       <c r="A68" s="12" t="s">
         <v>1109</v>
       </c>
@@ -35561,7 +35567,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="45">
+    <row r="70" spans="1:3" ht="43.2">
       <c r="A70" s="9" t="s">
         <v>1111</v>
       </c>
@@ -35572,7 +35578,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="45">
+    <row r="71" spans="1:3" ht="43.2">
       <c r="A71" s="9" t="s">
         <v>1112</v>
       </c>
@@ -35583,7 +35589,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="45">
+    <row r="72" spans="1:3" ht="43.2">
       <c r="A72" s="9" t="s">
         <v>1113</v>
       </c>
@@ -35594,7 +35600,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="45">
+    <row r="73" spans="1:3" ht="43.2">
       <c r="A73" s="9" t="s">
         <v>1114</v>
       </c>
@@ -35605,7 +35611,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="45">
+    <row r="74" spans="1:3" ht="43.2">
       <c r="A74" s="9" t="s">
         <v>1115</v>
       </c>
@@ -35616,7 +35622,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="45">
+    <row r="75" spans="1:3" ht="43.2">
       <c r="A75" s="9" t="s">
         <v>1116</v>
       </c>
@@ -35627,7 +35633,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="45">
+    <row r="76" spans="1:3" ht="43.2">
       <c r="A76" s="9" t="s">
         <v>1117</v>
       </c>
@@ -35638,7 +35644,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="45">
+    <row r="77" spans="1:3" ht="43.2">
       <c r="A77" s="9" t="s">
         <v>1118</v>
       </c>
@@ -35649,7 +35655,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="45">
+    <row r="78" spans="1:3" ht="43.2">
       <c r="A78" s="9" t="s">
         <v>1119</v>
       </c>
@@ -35660,7 +35666,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="45">
+    <row r="79" spans="1:3" ht="43.2">
       <c r="A79" s="9" t="s">
         <v>1120</v>
       </c>
@@ -35671,7 +35677,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="45">
+    <row r="80" spans="1:3" ht="43.2">
       <c r="A80" s="9" t="s">
         <v>1121</v>
       </c>
@@ -35682,7 +35688,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="45">
+    <row r="81" spans="1:3" ht="43.2">
       <c r="A81" s="9" t="s">
         <v>1122</v>
       </c>
@@ -35693,7 +35699,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="45">
+    <row r="82" spans="1:3" ht="43.2">
       <c r="A82" s="9" t="s">
         <v>1123</v>
       </c>
@@ -35704,7 +35710,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="45">
+    <row r="83" spans="1:3" ht="43.2">
       <c r="A83" s="9" t="s">
         <v>1124</v>
       </c>
@@ -35715,7 +35721,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="45">
+    <row r="84" spans="1:3" ht="43.2">
       <c r="A84" s="9" t="s">
         <v>1125</v>
       </c>
@@ -35726,7 +35732,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="45">
+    <row r="85" spans="1:3" ht="43.2">
       <c r="A85" s="9" t="s">
         <v>1126</v>
       </c>
@@ -35737,7 +35743,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="45">
+    <row r="86" spans="1:3" ht="43.2">
       <c r="A86" s="9" t="s">
         <v>1127</v>
       </c>
@@ -35748,7 +35754,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="45">
+    <row r="87" spans="1:3" ht="43.2">
       <c r="A87" s="9" t="s">
         <v>1128</v>
       </c>
@@ -35759,7 +35765,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="45">
+    <row r="88" spans="1:3" ht="43.2">
       <c r="A88" s="9" t="s">
         <v>1129</v>
       </c>
@@ -35770,7 +35776,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="45">
+    <row r="89" spans="1:3" ht="43.2">
       <c r="A89" s="9" t="s">
         <v>1130</v>
       </c>
@@ -35781,7 +35787,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="45">
+    <row r="90" spans="1:3" ht="43.2">
       <c r="A90" s="9" t="s">
         <v>1131</v>
       </c>
@@ -35792,7 +35798,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="45">
+    <row r="91" spans="1:3" ht="43.2">
       <c r="A91" s="9" t="s">
         <v>1132</v>
       </c>
@@ -35803,7 +35809,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="45">
+    <row r="92" spans="1:3" ht="43.2">
       <c r="A92" s="9" t="s">
         <v>1133</v>
       </c>
@@ -35814,7 +35820,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="45">
+    <row r="93" spans="1:3" ht="43.2">
       <c r="A93" s="9" t="s">
         <v>1134</v>
       </c>
@@ -35825,7 +35831,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="45">
+    <row r="94" spans="1:3" ht="43.2">
       <c r="A94" s="9" t="s">
         <v>1135</v>
       </c>
@@ -35836,7 +35842,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="45">
+    <row r="95" spans="1:3" ht="43.2">
       <c r="A95" s="9" t="s">
         <v>1136</v>
       </c>
@@ -35847,7 +35853,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="45">
+    <row r="96" spans="1:3" ht="43.2">
       <c r="A96" s="9" t="s">
         <v>1137</v>
       </c>
@@ -35858,7 +35864,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="45">
+    <row r="97" spans="1:3" ht="43.2">
       <c r="A97" s="9" t="s">
         <v>1138</v>
       </c>
@@ -35869,7 +35875,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="45">
+    <row r="98" spans="1:3" ht="43.2">
       <c r="A98" s="9" t="s">
         <v>1139</v>
       </c>
@@ -35913,7 +35919,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="45">
+    <row r="102" spans="1:3" ht="43.2">
       <c r="A102" s="9" t="s">
         <v>1143</v>
       </c>
@@ -36045,7 +36051,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="30">
+    <row r="114" spans="1:3" ht="28.8">
       <c r="A114" s="12" t="s">
         <v>1157</v>
       </c>
@@ -36056,7 +36062,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="30">
+    <row r="115" spans="1:3" ht="28.8">
       <c r="A115" s="12" t="s">
         <v>1158</v>
       </c>
@@ -36067,7 +36073,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="30">
+    <row r="116" spans="1:3" ht="28.8">
       <c r="A116" s="12" t="s">
         <v>1159</v>
       </c>
@@ -36078,7 +36084,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="30">
+    <row r="117" spans="1:3" ht="28.8">
       <c r="A117" s="12" t="s">
         <v>1160</v>
       </c>
@@ -36089,7 +36095,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="30">
+    <row r="118" spans="1:3" ht="28.8">
       <c r="A118" s="12" t="s">
         <v>1161</v>
       </c>
@@ -36100,7 +36106,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="30">
+    <row r="119" spans="1:3" ht="28.8">
       <c r="A119" s="12" t="s">
         <v>1162</v>
       </c>
@@ -36111,7 +36117,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="30">
+    <row r="120" spans="1:3" ht="28.8">
       <c r="A120" s="12" t="s">
         <v>1163</v>
       </c>
@@ -36122,7 +36128,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="30">
+    <row r="121" spans="1:3" ht="28.8">
       <c r="A121" s="12" t="s">
         <v>1164</v>
       </c>
@@ -36133,7 +36139,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="30">
+    <row r="122" spans="1:3" ht="28.8">
       <c r="A122" s="12" t="s">
         <v>1165</v>
       </c>
@@ -36144,7 +36150,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="30">
+    <row r="123" spans="1:3" ht="28.8">
       <c r="A123" s="12" t="s">
         <v>1166</v>
       </c>
@@ -36155,7 +36161,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="30">
+    <row r="124" spans="1:3" ht="28.8">
       <c r="A124" s="12" t="s">
         <v>1167</v>
       </c>
@@ -36166,7 +36172,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="30">
+    <row r="125" spans="1:3" ht="28.8">
       <c r="A125" s="12" t="s">
         <v>1168</v>
       </c>
@@ -36210,7 +36216,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="30">
+    <row r="129" spans="1:3" ht="28.8">
       <c r="A129" s="12" t="s">
         <v>1171</v>
       </c>
@@ -36221,7 +36227,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="30">
+    <row r="130" spans="1:3" ht="28.8">
       <c r="A130" s="12" t="s">
         <v>1172</v>
       </c>
@@ -36232,7 +36238,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="30">
+    <row r="131" spans="1:3" ht="28.8">
       <c r="A131" s="12" t="s">
         <v>1173</v>
       </c>
@@ -36287,7 +36293,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="30">
+    <row r="136" spans="1:3" ht="28.8">
       <c r="A136" s="12" t="s">
         <v>1174</v>
       </c>
@@ -36298,7 +36304,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="30">
+    <row r="137" spans="1:3" ht="28.8">
       <c r="A137" s="12" t="s">
         <v>1175</v>
       </c>
@@ -36309,7 +36315,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="30">
+    <row r="138" spans="1:3" ht="28.8">
       <c r="A138" s="12" t="s">
         <v>1176</v>
       </c>
@@ -36320,7 +36326,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="30">
+    <row r="139" spans="1:3" ht="28.8">
       <c r="A139" s="12" t="s">
         <v>1177</v>
       </c>
@@ -36331,7 +36337,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="30">
+    <row r="140" spans="1:3" ht="28.8">
       <c r="A140" s="12" t="s">
         <v>1178</v>
       </c>
@@ -36342,7 +36348,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="30">
+    <row r="141" spans="1:3" ht="28.8">
       <c r="A141" s="12" t="s">
         <v>1179</v>
       </c>
@@ -36353,7 +36359,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="30">
+    <row r="142" spans="1:3" ht="28.8">
       <c r="A142" s="12" t="s">
         <v>1180</v>
       </c>
@@ -36375,7 +36381,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="60">
+    <row r="144" spans="1:3" ht="43.2">
       <c r="A144" s="12" t="s">
         <v>1182</v>
       </c>
@@ -36386,7 +36392,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="60">
+    <row r="145" spans="1:3" ht="43.2">
       <c r="A145" s="12" t="s">
         <v>1183</v>
       </c>
@@ -36397,7 +36403,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="45">
+    <row r="146" spans="1:3" ht="43.2">
       <c r="A146" s="12" t="s">
         <v>1184</v>
       </c>
@@ -36408,7 +36414,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="45">
+    <row r="147" spans="1:3" ht="43.2">
       <c r="A147" s="12" t="s">
         <v>1185</v>
       </c>
@@ -36419,7 +36425,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="45">
+    <row r="148" spans="1:3" ht="43.2">
       <c r="A148" s="12" t="s">
         <v>1186</v>
       </c>
@@ -36430,7 +36436,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="45">
+    <row r="149" spans="1:3" ht="43.2">
       <c r="A149" s="12" t="s">
         <v>1187</v>
       </c>
@@ -36441,7 +36447,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="45">
+    <row r="150" spans="1:3" ht="43.2">
       <c r="A150" s="12" t="s">
         <v>1188</v>
       </c>
@@ -36474,7 +36480,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="45">
+    <row r="153" spans="1:3" ht="43.2">
       <c r="A153" s="12" t="s">
         <v>1191</v>
       </c>
@@ -36485,7 +36491,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="45">
+    <row r="154" spans="1:3" ht="43.2">
       <c r="A154" s="12" t="s">
         <v>1192</v>
       </c>
@@ -36496,7 +36502,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="30">
+    <row r="155" spans="1:3" ht="28.8">
       <c r="A155" s="12" t="s">
         <v>1194</v>
       </c>
@@ -36507,7 +36513,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="30">
+    <row r="156" spans="1:3" ht="28.8">
       <c r="A156" s="12" t="s">
         <v>1195</v>
       </c>
@@ -36518,7 +36524,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="30">
+    <row r="157" spans="1:3" ht="28.8">
       <c r="A157" s="12" t="s">
         <v>1196</v>
       </c>
@@ -36529,7 +36535,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="30">
+    <row r="158" spans="1:3" ht="28.8">
       <c r="A158" s="12" t="s">
         <v>1197</v>
       </c>
@@ -36540,7 +36546,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="30">
+    <row r="159" spans="1:3" ht="28.8">
       <c r="A159" s="12" t="s">
         <v>1198</v>
       </c>
@@ -36551,7 +36557,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="30">
+    <row r="160" spans="1:3" ht="28.8">
       <c r="A160" s="12" t="s">
         <v>1200</v>
       </c>
@@ -36562,7 +36568,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="30">
+    <row r="161" spans="1:3" ht="28.8">
       <c r="A161" s="12" t="s">
         <v>1201</v>
       </c>
@@ -36573,7 +36579,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="30">
+    <row r="162" spans="1:3" ht="28.8">
       <c r="A162" s="12" t="s">
         <v>1202</v>
       </c>
@@ -36584,7 +36590,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="30">
+    <row r="163" spans="1:3" ht="28.8">
       <c r="A163" s="12" t="s">
         <v>1203</v>
       </c>
@@ -36595,7 +36601,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="30">
+    <row r="164" spans="1:3" ht="28.8">
       <c r="A164" s="12" t="s">
         <v>1204</v>
       </c>
@@ -36606,7 +36612,7 @@
         <v>1273</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="30">
+    <row r="165" spans="1:3">
       <c r="A165" s="12" t="s">
         <v>1205</v>
       </c>
@@ -36617,7 +36623,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="45">
+    <row r="166" spans="1:3" ht="28.8">
       <c r="A166" s="12" t="s">
         <v>1206</v>
       </c>
@@ -36628,7 +36634,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="45">
+    <row r="167" spans="1:3" ht="28.8">
       <c r="A167" s="12" t="s">
         <v>1207</v>
       </c>
@@ -36639,7 +36645,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="45">
+    <row r="168" spans="1:3" ht="28.8">
       <c r="A168" s="12" t="s">
         <v>1208</v>
       </c>
@@ -36650,7 +36656,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="45">
+    <row r="169" spans="1:3" ht="28.8">
       <c r="A169" s="12" t="s">
         <v>1209</v>
       </c>
@@ -36661,7 +36667,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="45">
+    <row r="170" spans="1:3" ht="28.8">
       <c r="A170" s="12" t="s">
         <v>1210</v>
       </c>
@@ -36672,7 +36678,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="45">
+    <row r="171" spans="1:3" ht="28.8">
       <c r="A171" s="12" t="s">
         <v>1211</v>
       </c>
@@ -36683,7 +36689,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="30">
+    <row r="172" spans="1:3" ht="28.8">
       <c r="A172" s="12" t="s">
         <v>1213</v>
       </c>
@@ -36694,7 +36700,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="30">
+    <row r="173" spans="1:3" ht="28.8">
       <c r="A173" s="12" t="s">
         <v>1214</v>
       </c>
@@ -36705,7 +36711,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="30">
+    <row r="174" spans="1:3" ht="28.8">
       <c r="A174" s="12" t="s">
         <v>1215</v>
       </c>
@@ -36716,7 +36722,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="30">
+    <row r="175" spans="1:3" ht="28.8">
       <c r="A175" s="12" t="s">
         <v>1216</v>
       </c>
@@ -36727,7 +36733,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="30">
+    <row r="176" spans="1:3" ht="28.8">
       <c r="A176" s="12" t="s">
         <v>1217</v>
       </c>
@@ -36738,7 +36744,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="30">
+    <row r="177" spans="1:3" ht="28.8">
       <c r="A177" s="12" t="s">
         <v>1218</v>
       </c>
@@ -36749,7 +36755,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="30">
+    <row r="178" spans="1:3" ht="28.8">
       <c r="A178" s="12" t="s">
         <v>1219</v>
       </c>
@@ -36815,7 +36821,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="45">
+    <row r="184" spans="1:3" ht="28.8">
       <c r="A184" s="12" t="s">
         <v>1227</v>
       </c>
@@ -36826,7 +36832,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="45">
+    <row r="185" spans="1:3" ht="28.8">
       <c r="A185" s="12" t="s">
         <v>1228</v>
       </c>
@@ -36837,7 +36843,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="45">
+    <row r="186" spans="1:3" ht="28.8">
       <c r="A186" s="12" t="s">
         <v>1229</v>
       </c>
@@ -36848,7 +36854,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="187" spans="1:3" ht="45">
+    <row r="187" spans="1:3" ht="28.8">
       <c r="A187" s="12" t="s">
         <v>1230</v>
       </c>
@@ -36859,7 +36865,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="188" spans="1:3" ht="45">
+    <row r="188" spans="1:3" ht="28.8">
       <c r="A188" s="12" t="s">
         <v>1231</v>
       </c>
@@ -36870,7 +36876,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="45">
+    <row r="189" spans="1:3" ht="28.8">
       <c r="A189" s="12" t="s">
         <v>1232</v>
       </c>
@@ -36881,7 +36887,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="45">
+    <row r="190" spans="1:3" ht="43.2">
       <c r="A190" t="s">
         <v>1332</v>
       </c>
@@ -36892,7 +36898,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="45">
+    <row r="191" spans="1:3" ht="43.2">
       <c r="A191" t="s">
         <v>1333</v>
       </c>
@@ -36903,7 +36909,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="45">
+    <row r="192" spans="1:3" ht="43.2">
       <c r="A192" t="s">
         <v>1334</v>
       </c>
@@ -36914,7 +36920,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="45">
+    <row r="193" spans="1:3" ht="43.2">
       <c r="A193" t="s">
         <v>1335</v>
       </c>
@@ -36925,7 +36931,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="45">
+    <row r="194" spans="1:3" ht="43.2">
       <c r="A194" t="s">
         <v>1336</v>
       </c>
@@ -36936,7 +36942,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="45">
+    <row r="195" spans="1:3" ht="43.2">
       <c r="A195" t="s">
         <v>1337</v>
       </c>
@@ -36947,7 +36953,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="45">
+    <row r="196" spans="1:3" ht="43.2">
       <c r="A196" t="s">
         <v>1338</v>
       </c>
@@ -36958,7 +36964,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="45">
+    <row r="197" spans="1:3" ht="43.2">
       <c r="A197" t="s">
         <v>1339</v>
       </c>
@@ -36980,7 +36986,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="45">
+    <row r="199" spans="1:3" ht="43.2">
       <c r="A199" t="s">
         <v>1341</v>
       </c>
@@ -36991,7 +36997,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="45">
+    <row r="200" spans="1:3" ht="43.2">
       <c r="A200" t="s">
         <v>1342</v>
       </c>
@@ -37002,7 +37008,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="45">
+    <row r="201" spans="1:3" ht="43.2">
       <c r="A201" t="s">
         <v>1343</v>
       </c>
@@ -37057,7 +37063,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="30">
+    <row r="206" spans="1:3" ht="28.8">
       <c r="A206" s="4" t="s">
         <v>1397</v>
       </c>
@@ -37244,7 +37250,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="45">
+    <row r="223" spans="1:3" ht="28.8">
       <c r="A223" s="4" t="s">
         <v>1452</v>
       </c>
@@ -37255,7 +37261,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="45">
+    <row r="224" spans="1:3" ht="28.8">
       <c r="A224" s="15" t="s">
         <v>1453</v>
       </c>
@@ -37277,7 +37283,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="226" spans="1:3" ht="30">
+    <row r="226" spans="1:3" ht="28.8">
       <c r="A226" s="15" t="s">
         <v>1456</v>
       </c>
@@ -37288,7 +37294,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="227" spans="1:3" ht="30">
+    <row r="227" spans="1:3" ht="28.8">
       <c r="A227" s="4" t="s">
         <v>1457</v>
       </c>
@@ -37299,7 +37305,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="228" spans="1:3" ht="30">
+    <row r="228" spans="1:3" ht="28.8">
       <c r="A228" s="15" t="s">
         <v>1458</v>
       </c>
@@ -37310,7 +37316,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="229" spans="1:3" ht="30">
+    <row r="229" spans="1:3" ht="28.8">
       <c r="A229" s="15" t="s">
         <v>1459</v>
       </c>
@@ -37321,7 +37327,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="230" spans="1:3" ht="30">
+    <row r="230" spans="1:3" ht="28.8">
       <c r="A230" s="4" t="s">
         <v>1460</v>
       </c>
@@ -37332,7 +37338,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="231" spans="1:3" ht="30">
+    <row r="231" spans="1:3" ht="28.8">
       <c r="A231" s="4" t="s">
         <v>1461</v>
       </c>
@@ -37343,7 +37349,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="232" spans="1:3" ht="30">
+    <row r="232" spans="1:3" ht="28.8">
       <c r="A232" s="4" t="s">
         <v>1462</v>
       </c>
@@ -37398,7 +37404,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="237" spans="1:3" ht="30">
+    <row r="237" spans="1:3">
       <c r="A237" s="4" t="s">
         <v>1526</v>
       </c>
@@ -37409,7 +37415,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="238" spans="1:3" ht="30">
+    <row r="238" spans="1:3">
       <c r="A238" s="15" t="s">
         <v>1527</v>
       </c>

</xml_diff>

<commit_message>
Riders of Eomer and Paths of the Druadan
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F291B5-E943-4FBB-9553-4A77355F94DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CE0DB8-61E1-47F8-934E-C8AC8BE4FF40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">hero_constraints!$A$1:$C$262</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$J$460</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$H$738</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$J$477</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$H$774</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6907" uniqueCount="1878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7210" uniqueCount="1936">
   <si>
     <t>faction</t>
   </si>
@@ -5811,6 +5811,180 @@
   </si>
   <si>
     <t>["[theodred's_guard] theodred"]</t>
+  </si>
+  <si>
+    <t>OPT0760</t>
+  </si>
+  <si>
+    <t>OPT0761</t>
+  </si>
+  <si>
+    <t>OPT0762</t>
+  </si>
+  <si>
+    <t>OPT0763</t>
+  </si>
+  <si>
+    <t>OPT0764</t>
+  </si>
+  <si>
+    <t>OPT0765</t>
+  </si>
+  <si>
+    <t>OPT0766</t>
+  </si>
+  <si>
+    <t>OPT0767</t>
+  </si>
+  <si>
+    <t>OPT0768</t>
+  </si>
+  <si>
+    <t>OPT0769</t>
+  </si>
+  <si>
+    <t>OPT0770</t>
+  </si>
+  <si>
+    <t>OPT0771</t>
+  </si>
+  <si>
+    <t>OPT0772</t>
+  </si>
+  <si>
+    <t>OPT0773</t>
+  </si>
+  <si>
+    <t>[riders_of_eomer] erkenbrand</t>
+  </si>
+  <si>
+    <t>[riders_of_eomer] captain_of_rohan</t>
+  </si>
+  <si>
+    <t>[riders_of_eomer] eomer</t>
+  </si>
+  <si>
+    <t>[riders_of_eomer] gandalf_the_white</t>
+  </si>
+  <si>
+    <t>["[riders_of_eomer] rider_of_rohan"]</t>
+  </si>
+  <si>
+    <t>This force must contain Eomer.</t>
+  </si>
+  <si>
+    <t>["[riders_of_eomer] eomer"]</t>
+  </si>
+  <si>
+    <t>OPT0774</t>
+  </si>
+  <si>
+    <t>OPT0775</t>
+  </si>
+  <si>
+    <t>OPT0776</t>
+  </si>
+  <si>
+    <t>OPT0777</t>
+  </si>
+  <si>
+    <t>OPT0778</t>
+  </si>
+  <si>
+    <t>OPT0779</t>
+  </si>
+  <si>
+    <t>OPT0780</t>
+  </si>
+  <si>
+    <t>OPT0781</t>
+  </si>
+  <si>
+    <t>OPT0782</t>
+  </si>
+  <si>
+    <t>OPT0783</t>
+  </si>
+  <si>
+    <t>OPT0784</t>
+  </si>
+  <si>
+    <t>OPT0785</t>
+  </si>
+  <si>
+    <t>OPT0786</t>
+  </si>
+  <si>
+    <t>OPT0787</t>
+  </si>
+  <si>
+    <t>OPT0788</t>
+  </si>
+  <si>
+    <t>OPT0789</t>
+  </si>
+  <si>
+    <t>OPT0790</t>
+  </si>
+  <si>
+    <t>OPT0791</t>
+  </si>
+  <si>
+    <t>OPT0792</t>
+  </si>
+  <si>
+    <t>OPT0793</t>
+  </si>
+  <si>
+    <t>OPT0794</t>
+  </si>
+  <si>
+    <t>OPT0795</t>
+  </si>
+  <si>
+    <t>OPT0796</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] deorwine</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] elfhelm</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] gamling</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] captain_of_rohan</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] theoden</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] eomer</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] dernhelm</t>
+  </si>
+  <si>
+    <t>[paths_of_the_druadan] ghan-buri-ghan</t>
+  </si>
+  <si>
+    <t>['[paths_of_the_druadan] rider_of_rohan', '[paths_of_the_druadan] rohan_royal_guard', '[paths_of_the_druadan] rohan_outrider']</t>
+  </si>
+  <si>
+    <t>['[paths_of_the_druadan] woses_warrior']</t>
+  </si>
+  <si>
+    <t>['[paths_of_the_druadan] theoden']</t>
+  </si>
+  <si>
+    <t>['[paths_of_the_druadan] ghan-buri-ghan']</t>
+  </si>
+  <si>
+    <t>This force must contain Ghan-Buri-Ghan.</t>
+  </si>
+  <si>
+    <t>Ghan-Buri-Ghan's warband must contain a full warband of Woses Warriors.</t>
   </si>
 </sst>
 </file>
@@ -6313,11 +6487,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J460"/>
+  <dimension ref="A1:J477"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A456" sqref="A456"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A466" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E485" sqref="E485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21246,7 +21420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:10">
+    <row r="453" spans="1:10" hidden="1">
       <c r="A453" s="15" t="str">
         <f t="shared" si="7"/>
         <v>[theodred's_guard] elfhelm</v>
@@ -21279,7 +21453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:10">
+    <row r="454" spans="1:10" hidden="1">
       <c r="A454" s="15" t="str">
         <f t="shared" si="7"/>
         <v>[theodred's_guard] grimbold</v>
@@ -21312,7 +21486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="455" spans="1:10">
+    <row r="455" spans="1:10" hidden="1">
       <c r="A455" s="15" t="str">
         <f t="shared" si="7"/>
         <v>[theodred's_guard] captain_of_rohan</v>
@@ -21345,9 +21519,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:10">
+    <row r="456" spans="1:10" hidden="1">
       <c r="A456" s="15" t="str">
-        <f t="shared" ref="A456:A460" si="8">_xlfn.CONCAT("[", LOWER(SUBSTITUTE(C456, " ", "_")), "] ", LOWER(SUBSTITUTE(E456, " ", "_")))</f>
+        <f t="shared" ref="A456:A477" si="8">_xlfn.CONCAT("[", LOWER(SUBSTITUTE(C456, " ", "_")), "] ", LOWER(SUBSTITUTE(E456, " ", "_")))</f>
         <v>[theodred's_guard] theodred</v>
       </c>
       <c r="B456" t="s">
@@ -21378,7 +21552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:10">
+    <row r="457" spans="1:10" hidden="1">
       <c r="A457" s="15" t="str">
         <f t="shared" si="8"/>
         <v>[theodred's_guard] rider_of_rohan</v>
@@ -21411,7 +21585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:10">
+    <row r="458" spans="1:10" hidden="1">
       <c r="A458" s="15" t="str">
         <f t="shared" si="8"/>
         <v>[theodred's_guard] rohan_royal_guard</v>
@@ -21444,7 +21618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="459" spans="1:10">
+    <row r="459" spans="1:10" hidden="1">
       <c r="A459" s="15" t="str">
         <f t="shared" si="8"/>
         <v>[theodred's_guard] rohan_outrider</v>
@@ -21477,7 +21651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:10">
+    <row r="460" spans="1:10" hidden="1">
       <c r="A460" s="15" t="str">
         <f t="shared" si="8"/>
         <v>[theodred's_guard] warrior_of_rohan</v>
@@ -21510,11 +21684,572 @@
         <v>0</v>
       </c>
     </row>
+    <row r="461" spans="1:10" hidden="1">
+      <c r="A461" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[riders_of_eomer] erkenbrand</v>
+      </c>
+      <c r="B461" t="s">
+        <v>211</v>
+      </c>
+      <c r="C461" t="s">
+        <v>860</v>
+      </c>
+      <c r="D461" t="s">
+        <v>132</v>
+      </c>
+      <c r="E461" t="s">
+        <v>163</v>
+      </c>
+      <c r="F461" t="s">
+        <v>10</v>
+      </c>
+      <c r="G461">
+        <v>85</v>
+      </c>
+      <c r="H461" t="b">
+        <v>0</v>
+      </c>
+      <c r="I461" t="b">
+        <v>1</v>
+      </c>
+      <c r="J461">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" hidden="1">
+      <c r="A462" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[riders_of_eomer] captain_of_rohan</v>
+      </c>
+      <c r="B462" t="s">
+        <v>211</v>
+      </c>
+      <c r="C462" t="s">
+        <v>860</v>
+      </c>
+      <c r="D462" t="s">
+        <v>132</v>
+      </c>
+      <c r="E462" t="s">
+        <v>159</v>
+      </c>
+      <c r="F462" t="s">
+        <v>10</v>
+      </c>
+      <c r="G462">
+        <v>55</v>
+      </c>
+      <c r="H462" t="b">
+        <v>0</v>
+      </c>
+      <c r="I462" t="b">
+        <v>0</v>
+      </c>
+      <c r="J462">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" hidden="1">
+      <c r="A463" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[riders_of_eomer] eomer</v>
+      </c>
+      <c r="B463" t="s">
+        <v>211</v>
+      </c>
+      <c r="C463" t="s">
+        <v>860</v>
+      </c>
+      <c r="D463" t="s">
+        <v>132</v>
+      </c>
+      <c r="E463" t="s">
+        <v>134</v>
+      </c>
+      <c r="F463" t="s">
+        <v>7</v>
+      </c>
+      <c r="G463">
+        <v>110</v>
+      </c>
+      <c r="H463" t="b">
+        <v>0</v>
+      </c>
+      <c r="I463" t="b">
+        <v>1</v>
+      </c>
+      <c r="J463">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="464" spans="1:10" hidden="1">
+      <c r="A464" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[riders_of_eomer] rider_of_rohan</v>
+      </c>
+      <c r="B464" t="s">
+        <v>211</v>
+      </c>
+      <c r="C464" t="s">
+        <v>860</v>
+      </c>
+      <c r="D464" t="s">
+        <v>132</v>
+      </c>
+      <c r="E464" t="s">
+        <v>137</v>
+      </c>
+      <c r="F464" t="s">
+        <v>12</v>
+      </c>
+      <c r="G464">
+        <v>14</v>
+      </c>
+      <c r="H464" t="b">
+        <v>0</v>
+      </c>
+      <c r="I464" t="b">
+        <v>0</v>
+      </c>
+      <c r="J464">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="465" spans="1:10" hidden="1">
+      <c r="A465" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[riders_of_eomer] gandalf_the_white</v>
+      </c>
+      <c r="B465" t="s">
+        <v>211</v>
+      </c>
+      <c r="C465" t="s">
+        <v>860</v>
+      </c>
+      <c r="D465" t="s">
+        <v>71</v>
+      </c>
+      <c r="E465" t="s">
+        <v>83</v>
+      </c>
+      <c r="F465" t="s">
+        <v>7</v>
+      </c>
+      <c r="G465">
+        <v>240</v>
+      </c>
+      <c r="H465" t="b">
+        <v>0</v>
+      </c>
+      <c r="I465" t="b">
+        <v>1</v>
+      </c>
+      <c r="J465">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="466" spans="1:10">
+      <c r="A466" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] deorwine</v>
+      </c>
+      <c r="B466" t="s">
+        <v>211</v>
+      </c>
+      <c r="C466" t="s">
+        <v>917</v>
+      </c>
+      <c r="D466" t="s">
+        <v>132</v>
+      </c>
+      <c r="E466" t="s">
+        <v>160</v>
+      </c>
+      <c r="F466" t="s">
+        <v>10</v>
+      </c>
+      <c r="G466">
+        <v>85</v>
+      </c>
+      <c r="H466" t="b">
+        <v>0</v>
+      </c>
+      <c r="I466" t="b">
+        <v>1</v>
+      </c>
+      <c r="J466">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="467" spans="1:10">
+      <c r="A467" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] elfhelm</v>
+      </c>
+      <c r="B467" t="s">
+        <v>211</v>
+      </c>
+      <c r="C467" t="s">
+        <v>917</v>
+      </c>
+      <c r="D467" t="s">
+        <v>132</v>
+      </c>
+      <c r="E467" t="s">
+        <v>161</v>
+      </c>
+      <c r="F467" t="s">
+        <v>10</v>
+      </c>
+      <c r="G467">
+        <v>75</v>
+      </c>
+      <c r="H467" t="b">
+        <v>0</v>
+      </c>
+      <c r="I467" t="b">
+        <v>1</v>
+      </c>
+      <c r="J467">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10">
+      <c r="A468" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] gamling</v>
+      </c>
+      <c r="B468" t="s">
+        <v>211</v>
+      </c>
+      <c r="C468" t="s">
+        <v>917</v>
+      </c>
+      <c r="D468" t="s">
+        <v>132</v>
+      </c>
+      <c r="E468" t="s">
+        <v>135</v>
+      </c>
+      <c r="F468" t="s">
+        <v>10</v>
+      </c>
+      <c r="G468">
+        <v>65</v>
+      </c>
+      <c r="H468" t="b">
+        <v>0</v>
+      </c>
+      <c r="I468" t="b">
+        <v>1</v>
+      </c>
+      <c r="J468">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10">
+      <c r="A469" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] captain_of_rohan</v>
+      </c>
+      <c r="B469" t="s">
+        <v>211</v>
+      </c>
+      <c r="C469" t="s">
+        <v>917</v>
+      </c>
+      <c r="D469" t="s">
+        <v>132</v>
+      </c>
+      <c r="E469" t="s">
+        <v>159</v>
+      </c>
+      <c r="F469" t="s">
+        <v>10</v>
+      </c>
+      <c r="G469">
+        <v>55</v>
+      </c>
+      <c r="H469" t="b">
+        <v>0</v>
+      </c>
+      <c r="I469" t="b">
+        <v>0</v>
+      </c>
+      <c r="J469">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10">
+      <c r="A470" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] theoden</v>
+      </c>
+      <c r="B470" t="s">
+        <v>211</v>
+      </c>
+      <c r="C470" t="s">
+        <v>917</v>
+      </c>
+      <c r="D470" t="s">
+        <v>132</v>
+      </c>
+      <c r="E470" t="s">
+        <v>139</v>
+      </c>
+      <c r="F470" t="s">
+        <v>15</v>
+      </c>
+      <c r="G470">
+        <v>90</v>
+      </c>
+      <c r="H470" t="b">
+        <v>0</v>
+      </c>
+      <c r="I470" t="b">
+        <v>1</v>
+      </c>
+      <c r="J470">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10">
+      <c r="A471" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] eomer</v>
+      </c>
+      <c r="B471" t="s">
+        <v>211</v>
+      </c>
+      <c r="C471" t="s">
+        <v>917</v>
+      </c>
+      <c r="D471" t="s">
+        <v>132</v>
+      </c>
+      <c r="E471" t="s">
+        <v>134</v>
+      </c>
+      <c r="F471" t="s">
+        <v>7</v>
+      </c>
+      <c r="G471">
+        <v>115</v>
+      </c>
+      <c r="H471" t="b">
+        <v>0</v>
+      </c>
+      <c r="I471" t="b">
+        <v>1</v>
+      </c>
+      <c r="J471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10">
+      <c r="A472" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] dernhelm</v>
+      </c>
+      <c r="B472" t="s">
+        <v>211</v>
+      </c>
+      <c r="C472" t="s">
+        <v>917</v>
+      </c>
+      <c r="D472" t="s">
+        <v>132</v>
+      </c>
+      <c r="E472" t="s">
+        <v>133</v>
+      </c>
+      <c r="F472" t="s">
+        <v>22</v>
+      </c>
+      <c r="G472">
+        <v>75</v>
+      </c>
+      <c r="H472" t="b">
+        <v>0</v>
+      </c>
+      <c r="I472" t="b">
+        <v>1</v>
+      </c>
+      <c r="J472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10">
+      <c r="A473" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] rider_of_rohan</v>
+      </c>
+      <c r="B473" t="s">
+        <v>211</v>
+      </c>
+      <c r="C473" t="s">
+        <v>917</v>
+      </c>
+      <c r="D473" t="s">
+        <v>132</v>
+      </c>
+      <c r="E473" t="s">
+        <v>137</v>
+      </c>
+      <c r="F473" t="s">
+        <v>12</v>
+      </c>
+      <c r="G473">
+        <v>14</v>
+      </c>
+      <c r="H473" t="b">
+        <v>0</v>
+      </c>
+      <c r="I473" t="b">
+        <v>0</v>
+      </c>
+      <c r="J473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:10">
+      <c r="A474" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] rohan_royal_guard</v>
+      </c>
+      <c r="B474" t="s">
+        <v>211</v>
+      </c>
+      <c r="C474" t="s">
+        <v>917</v>
+      </c>
+      <c r="D474" t="s">
+        <v>132</v>
+      </c>
+      <c r="E474" t="s">
+        <v>138</v>
+      </c>
+      <c r="F474" t="s">
+        <v>12</v>
+      </c>
+      <c r="G474">
+        <v>15</v>
+      </c>
+      <c r="H474" t="b">
+        <v>0</v>
+      </c>
+      <c r="I474" t="b">
+        <v>0</v>
+      </c>
+      <c r="J474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10">
+      <c r="A475" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] rohan_outrider</v>
+      </c>
+      <c r="B475" t="s">
+        <v>211</v>
+      </c>
+      <c r="C475" t="s">
+        <v>917</v>
+      </c>
+      <c r="D475" t="s">
+        <v>132</v>
+      </c>
+      <c r="E475" t="s">
+        <v>176</v>
+      </c>
+      <c r="F475" t="s">
+        <v>12</v>
+      </c>
+      <c r="G475">
+        <v>13</v>
+      </c>
+      <c r="H475" t="b">
+        <v>1</v>
+      </c>
+      <c r="I475" t="b">
+        <v>0</v>
+      </c>
+      <c r="J475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:10">
+      <c r="A476" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] ghan-buri-ghan</v>
+      </c>
+      <c r="B476" t="s">
+        <v>211</v>
+      </c>
+      <c r="C476" t="s">
+        <v>917</v>
+      </c>
+      <c r="D476" t="s">
+        <v>915</v>
+      </c>
+      <c r="E476" t="s">
+        <v>1532</v>
+      </c>
+      <c r="F476" t="s">
+        <v>7</v>
+      </c>
+      <c r="G476">
+        <v>65</v>
+      </c>
+      <c r="H476" t="b">
+        <v>0</v>
+      </c>
+      <c r="I476" t="b">
+        <v>1</v>
+      </c>
+      <c r="J476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:10">
+      <c r="A477" s="15" t="str">
+        <f t="shared" si="8"/>
+        <v>[paths_of_the_druadan] woses_warrior</v>
+      </c>
+      <c r="B477" t="s">
+        <v>211</v>
+      </c>
+      <c r="C477" t="s">
+        <v>917</v>
+      </c>
+      <c r="D477" t="s">
+        <v>915</v>
+      </c>
+      <c r="E477" t="s">
+        <v>1554</v>
+      </c>
+      <c r="F477" t="s">
+        <v>12</v>
+      </c>
+      <c r="G477">
+        <v>9</v>
+      </c>
+      <c r="H477" t="b">
+        <v>0</v>
+      </c>
+      <c r="I477" t="b">
+        <v>0</v>
+      </c>
+      <c r="J477">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J460" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
+  <autoFilter ref="A1:J477" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Theodred's Guard"/>
+        <filter val="Paths of the Druadan"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -21530,11 +22265,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
-  <dimension ref="A1:H760"/>
+  <dimension ref="A1:H797"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A732" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D756" sqref="D756"/>
+      <pane ySplit="1" topLeftCell="A765" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A771" sqref="A771:A797"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39863,8 +40598,913 @@
         <v>1</v>
       </c>
     </row>
+    <row r="761" spans="1:8">
+      <c r="A761" s="5" t="s">
+        <v>1878</v>
+      </c>
+      <c r="B761" t="s">
+        <v>860</v>
+      </c>
+      <c r="C761" t="s">
+        <v>159</v>
+      </c>
+      <c r="D761" t="s">
+        <v>262</v>
+      </c>
+      <c r="E761">
+        <v>10</v>
+      </c>
+      <c r="F761" t="s">
+        <v>256</v>
+      </c>
+      <c r="G761">
+        <v>1</v>
+      </c>
+      <c r="H761">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="762" spans="1:8">
+      <c r="A762" s="5" t="s">
+        <v>1879</v>
+      </c>
+      <c r="B762" t="s">
+        <v>860</v>
+      </c>
+      <c r="C762" t="s">
+        <v>159</v>
+      </c>
+      <c r="D762" t="s">
+        <v>356</v>
+      </c>
+      <c r="E762">
+        <v>5</v>
+      </c>
+      <c r="F762" t="s">
+        <v>317</v>
+      </c>
+      <c r="G762">
+        <v>0</v>
+      </c>
+      <c r="H762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:8">
+      <c r="A763" s="5" t="s">
+        <v>1880</v>
+      </c>
+      <c r="B763" t="s">
+        <v>860</v>
+      </c>
+      <c r="C763" t="s">
+        <v>159</v>
+      </c>
+      <c r="D763" t="s">
+        <v>350</v>
+      </c>
+      <c r="E763">
+        <v>5</v>
+      </c>
+      <c r="F763" t="s">
+        <v>351</v>
+      </c>
+      <c r="G763">
+        <v>0</v>
+      </c>
+      <c r="H763">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="764" spans="1:8">
+      <c r="A764" s="5" t="s">
+        <v>1881</v>
+      </c>
+      <c r="B764" t="s">
+        <v>860</v>
+      </c>
+      <c r="C764" t="s">
+        <v>159</v>
+      </c>
+      <c r="D764" t="s">
+        <v>312</v>
+      </c>
+      <c r="E764">
+        <v>5</v>
+      </c>
+      <c r="G764">
+        <v>0</v>
+      </c>
+      <c r="H764">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="765" spans="1:8">
+      <c r="A765" s="5" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B765" t="s">
+        <v>860</v>
+      </c>
+      <c r="C765" t="s">
+        <v>159</v>
+      </c>
+      <c r="D765" t="s">
+        <v>332</v>
+      </c>
+      <c r="E765">
+        <v>5</v>
+      </c>
+      <c r="G765">
+        <v>0</v>
+      </c>
+      <c r="H765">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="766" spans="1:8">
+      <c r="A766" s="5" t="s">
+        <v>1883</v>
+      </c>
+      <c r="B766" t="s">
+        <v>860</v>
+      </c>
+      <c r="C766" t="s">
+        <v>134</v>
+      </c>
+      <c r="D766" t="s">
+        <v>262</v>
+      </c>
+      <c r="E766">
+        <v>10</v>
+      </c>
+      <c r="F766" t="s">
+        <v>256</v>
+      </c>
+      <c r="G766">
+        <v>1</v>
+      </c>
+      <c r="H766">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="767" spans="1:8">
+      <c r="A767" s="5" t="s">
+        <v>1884</v>
+      </c>
+      <c r="B767" t="s">
+        <v>860</v>
+      </c>
+      <c r="C767" t="s">
+        <v>134</v>
+      </c>
+      <c r="D767" t="s">
+        <v>312</v>
+      </c>
+      <c r="E767">
+        <v>5</v>
+      </c>
+      <c r="G767">
+        <v>0</v>
+      </c>
+      <c r="H767">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="768" spans="1:8">
+      <c r="A768" s="5" t="s">
+        <v>1885</v>
+      </c>
+      <c r="B768" t="s">
+        <v>860</v>
+      </c>
+      <c r="C768" t="s">
+        <v>134</v>
+      </c>
+      <c r="D768" t="s">
+        <v>332</v>
+      </c>
+      <c r="E768">
+        <v>5</v>
+      </c>
+      <c r="G768">
+        <v>0</v>
+      </c>
+      <c r="H768">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="769" spans="1:8">
+      <c r="A769" s="5" t="s">
+        <v>1886</v>
+      </c>
+      <c r="B769" t="s">
+        <v>860</v>
+      </c>
+      <c r="C769" t="s">
+        <v>163</v>
+      </c>
+      <c r="D769" t="s">
+        <v>262</v>
+      </c>
+      <c r="E769">
+        <v>10</v>
+      </c>
+      <c r="F769" t="s">
+        <v>256</v>
+      </c>
+      <c r="G769">
+        <v>1</v>
+      </c>
+      <c r="H769">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="770" spans="1:8">
+      <c r="A770" s="5" t="s">
+        <v>1887</v>
+      </c>
+      <c r="B770" t="s">
+        <v>860</v>
+      </c>
+      <c r="C770" t="s">
+        <v>137</v>
+      </c>
+      <c r="D770" t="s">
+        <v>284</v>
+      </c>
+      <c r="E770">
+        <v>30</v>
+      </c>
+      <c r="G770">
+        <v>0</v>
+      </c>
+      <c r="H770">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="771" spans="1:8">
+      <c r="A771" s="5" t="s">
+        <v>1888</v>
+      </c>
+      <c r="B771" t="s">
+        <v>860</v>
+      </c>
+      <c r="C771" t="s">
+        <v>137</v>
+      </c>
+      <c r="D771" t="s">
+        <v>286</v>
+      </c>
+      <c r="E771">
+        <v>25</v>
+      </c>
+      <c r="G771">
+        <v>0</v>
+      </c>
+      <c r="H771">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="772" spans="1:8">
+      <c r="A772" s="5" t="s">
+        <v>1889</v>
+      </c>
+      <c r="B772" t="s">
+        <v>860</v>
+      </c>
+      <c r="C772" t="s">
+        <v>137</v>
+      </c>
+      <c r="D772" t="s">
+        <v>332</v>
+      </c>
+      <c r="E772">
+        <v>2</v>
+      </c>
+      <c r="G772">
+        <v>0</v>
+      </c>
+      <c r="H772">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="773" spans="1:8">
+      <c r="A773" s="5" t="s">
+        <v>1890</v>
+      </c>
+      <c r="B773" t="s">
+        <v>860</v>
+      </c>
+      <c r="C773" t="s">
+        <v>137</v>
+      </c>
+      <c r="D773" t="s">
+        <v>1226</v>
+      </c>
+      <c r="E773">
+        <v>1</v>
+      </c>
+      <c r="F773" t="s">
+        <v>402</v>
+      </c>
+      <c r="G773">
+        <v>0</v>
+      </c>
+      <c r="H773">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="774" spans="1:8">
+      <c r="A774" s="5" t="s">
+        <v>1891</v>
+      </c>
+      <c r="B774" t="s">
+        <v>860</v>
+      </c>
+      <c r="C774" t="s">
+        <v>83</v>
+      </c>
+      <c r="D774" t="s">
+        <v>478</v>
+      </c>
+      <c r="E774">
+        <v>20</v>
+      </c>
+      <c r="F774" t="s">
+        <v>256</v>
+      </c>
+      <c r="G774">
+        <v>1</v>
+      </c>
+      <c r="H774">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="775" spans="1:8">
+      <c r="A775" s="5" t="s">
+        <v>1899</v>
+      </c>
+      <c r="B775" t="s">
+        <v>917</v>
+      </c>
+      <c r="C775" t="s">
+        <v>159</v>
+      </c>
+      <c r="D775" t="s">
+        <v>262</v>
+      </c>
+      <c r="E775">
+        <v>10</v>
+      </c>
+      <c r="F775" t="s">
+        <v>256</v>
+      </c>
+      <c r="G775">
+        <v>1</v>
+      </c>
+      <c r="H775">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="776" spans="1:8">
+      <c r="A776" s="5" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B776" t="s">
+        <v>917</v>
+      </c>
+      <c r="C776" t="s">
+        <v>159</v>
+      </c>
+      <c r="D776" t="s">
+        <v>356</v>
+      </c>
+      <c r="E776">
+        <v>5</v>
+      </c>
+      <c r="F776" t="s">
+        <v>317</v>
+      </c>
+      <c r="G776">
+        <v>0</v>
+      </c>
+      <c r="H776">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="777" spans="1:8">
+      <c r="A777" s="5" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B777" t="s">
+        <v>917</v>
+      </c>
+      <c r="C777" t="s">
+        <v>159</v>
+      </c>
+      <c r="D777" t="s">
+        <v>350</v>
+      </c>
+      <c r="E777">
+        <v>5</v>
+      </c>
+      <c r="F777" t="s">
+        <v>351</v>
+      </c>
+      <c r="G777">
+        <v>0</v>
+      </c>
+      <c r="H777">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:8">
+      <c r="A778" s="5" t="s">
+        <v>1902</v>
+      </c>
+      <c r="B778" t="s">
+        <v>917</v>
+      </c>
+      <c r="C778" t="s">
+        <v>159</v>
+      </c>
+      <c r="D778" t="s">
+        <v>312</v>
+      </c>
+      <c r="E778">
+        <v>5</v>
+      </c>
+      <c r="G778">
+        <v>0</v>
+      </c>
+      <c r="H778">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="779" spans="1:8">
+      <c r="A779" s="5" t="s">
+        <v>1903</v>
+      </c>
+      <c r="B779" t="s">
+        <v>917</v>
+      </c>
+      <c r="C779" t="s">
+        <v>159</v>
+      </c>
+      <c r="D779" t="s">
+        <v>332</v>
+      </c>
+      <c r="E779">
+        <v>5</v>
+      </c>
+      <c r="G779">
+        <v>0</v>
+      </c>
+      <c r="H779">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="780" spans="1:8">
+      <c r="A780" s="5" t="s">
+        <v>1904</v>
+      </c>
+      <c r="B780" t="s">
+        <v>917</v>
+      </c>
+      <c r="C780" t="s">
+        <v>160</v>
+      </c>
+      <c r="D780" t="s">
+        <v>262</v>
+      </c>
+      <c r="E780">
+        <v>10</v>
+      </c>
+      <c r="F780" t="s">
+        <v>256</v>
+      </c>
+      <c r="G780">
+        <v>1</v>
+      </c>
+      <c r="H780">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="781" spans="1:8">
+      <c r="A781" s="5" t="s">
+        <v>1905</v>
+      </c>
+      <c r="B781" t="s">
+        <v>917</v>
+      </c>
+      <c r="C781" t="s">
+        <v>133</v>
+      </c>
+      <c r="D781" t="s">
+        <v>332</v>
+      </c>
+      <c r="E781">
+        <v>5</v>
+      </c>
+      <c r="G781">
+        <v>0</v>
+      </c>
+      <c r="H781">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="782" spans="1:8">
+      <c r="A782" s="5" t="s">
+        <v>1906</v>
+      </c>
+      <c r="B782" t="s">
+        <v>917</v>
+      </c>
+      <c r="C782" t="s">
+        <v>161</v>
+      </c>
+      <c r="D782" t="s">
+        <v>262</v>
+      </c>
+      <c r="E782">
+        <v>10</v>
+      </c>
+      <c r="F782" t="s">
+        <v>256</v>
+      </c>
+      <c r="G782">
+        <v>1</v>
+      </c>
+      <c r="H782">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="783" spans="1:8">
+      <c r="A783" s="5" t="s">
+        <v>1907</v>
+      </c>
+      <c r="B783" t="s">
+        <v>917</v>
+      </c>
+      <c r="C783" t="s">
+        <v>134</v>
+      </c>
+      <c r="D783" t="s">
+        <v>260</v>
+      </c>
+      <c r="E783">
+        <v>15</v>
+      </c>
+      <c r="F783" t="s">
+        <v>256</v>
+      </c>
+      <c r="G783">
+        <v>1</v>
+      </c>
+      <c r="H783">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="784" spans="1:8">
+      <c r="A784" s="5" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B784" t="s">
+        <v>917</v>
+      </c>
+      <c r="C784" t="s">
+        <v>134</v>
+      </c>
+      <c r="D784" t="s">
+        <v>312</v>
+      </c>
+      <c r="E784">
+        <v>5</v>
+      </c>
+      <c r="G784">
+        <v>0</v>
+      </c>
+      <c r="H784">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="785" spans="1:8">
+      <c r="A785" s="5" t="s">
+        <v>1909</v>
+      </c>
+      <c r="B785" t="s">
+        <v>917</v>
+      </c>
+      <c r="C785" t="s">
+        <v>134</v>
+      </c>
+      <c r="D785" t="s">
+        <v>332</v>
+      </c>
+      <c r="E785">
+        <v>5</v>
+      </c>
+      <c r="G785">
+        <v>0</v>
+      </c>
+      <c r="H785">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="786" spans="1:8">
+      <c r="A786" s="5" t="s">
+        <v>1910</v>
+      </c>
+      <c r="B786" t="s">
+        <v>917</v>
+      </c>
+      <c r="C786" t="s">
+        <v>135</v>
+      </c>
+      <c r="D786" t="s">
+        <v>653</v>
+      </c>
+      <c r="E786">
+        <v>50</v>
+      </c>
+      <c r="G786">
+        <v>0</v>
+      </c>
+      <c r="H786">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="787" spans="1:8">
+      <c r="A787" s="5" t="s">
+        <v>1911</v>
+      </c>
+      <c r="B787" t="s">
+        <v>917</v>
+      </c>
+      <c r="C787" t="s">
+        <v>135</v>
+      </c>
+      <c r="D787" t="s">
+        <v>262</v>
+      </c>
+      <c r="E787">
+        <v>10</v>
+      </c>
+      <c r="F787" t="s">
+        <v>256</v>
+      </c>
+      <c r="G787">
+        <v>1</v>
+      </c>
+      <c r="H787">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="788" spans="1:8">
+      <c r="A788" s="5" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B788" t="s">
+        <v>917</v>
+      </c>
+      <c r="C788" t="s">
+        <v>137</v>
+      </c>
+      <c r="D788" t="s">
+        <v>284</v>
+      </c>
+      <c r="E788">
+        <v>30</v>
+      </c>
+      <c r="G788">
+        <v>0</v>
+      </c>
+      <c r="H788">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="789" spans="1:8">
+      <c r="A789" s="5" t="s">
+        <v>1913</v>
+      </c>
+      <c r="B789" t="s">
+        <v>917</v>
+      </c>
+      <c r="C789" t="s">
+        <v>137</v>
+      </c>
+      <c r="D789" t="s">
+        <v>286</v>
+      </c>
+      <c r="E789">
+        <v>25</v>
+      </c>
+      <c r="G789">
+        <v>0</v>
+      </c>
+      <c r="H789">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="790" spans="1:8">
+      <c r="A790" s="5" t="s">
+        <v>1914</v>
+      </c>
+      <c r="B790" t="s">
+        <v>917</v>
+      </c>
+      <c r="C790" t="s">
+        <v>137</v>
+      </c>
+      <c r="D790" t="s">
+        <v>332</v>
+      </c>
+      <c r="E790">
+        <v>2</v>
+      </c>
+      <c r="G790">
+        <v>0</v>
+      </c>
+      <c r="H790">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="791" spans="1:8">
+      <c r="A791" s="5" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B791" t="s">
+        <v>917</v>
+      </c>
+      <c r="C791" t="s">
+        <v>176</v>
+      </c>
+      <c r="D791" t="s">
+        <v>262</v>
+      </c>
+      <c r="E791">
+        <v>5</v>
+      </c>
+      <c r="F791" t="s">
+        <v>256</v>
+      </c>
+      <c r="G791">
+        <v>1</v>
+      </c>
+      <c r="H791">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="792" spans="1:8">
+      <c r="A792" s="5" t="s">
+        <v>1916</v>
+      </c>
+      <c r="B792" t="s">
+        <v>917</v>
+      </c>
+      <c r="C792" t="s">
+        <v>138</v>
+      </c>
+      <c r="D792" t="s">
+        <v>286</v>
+      </c>
+      <c r="E792">
+        <v>25</v>
+      </c>
+      <c r="G792">
+        <v>0</v>
+      </c>
+      <c r="H792">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="793" spans="1:8">
+      <c r="A793" s="5" t="s">
+        <v>1917</v>
+      </c>
+      <c r="B793" t="s">
+        <v>917</v>
+      </c>
+      <c r="C793" t="s">
+        <v>138</v>
+      </c>
+      <c r="D793" t="s">
+        <v>262</v>
+      </c>
+      <c r="E793">
+        <v>5</v>
+      </c>
+      <c r="F793" t="s">
+        <v>256</v>
+      </c>
+      <c r="G793">
+        <v>1</v>
+      </c>
+      <c r="H793">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="794" spans="1:8">
+      <c r="A794" s="5" t="s">
+        <v>1918</v>
+      </c>
+      <c r="B794" t="s">
+        <v>917</v>
+      </c>
+      <c r="C794" t="s">
+        <v>138</v>
+      </c>
+      <c r="D794" t="s">
+        <v>332</v>
+      </c>
+      <c r="E794">
+        <v>2</v>
+      </c>
+      <c r="G794">
+        <v>0</v>
+      </c>
+      <c r="H794">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="795" spans="1:8">
+      <c r="A795" s="5" t="s">
+        <v>1919</v>
+      </c>
+      <c r="B795" t="s">
+        <v>917</v>
+      </c>
+      <c r="C795" t="s">
+        <v>139</v>
+      </c>
+      <c r="D795" t="s">
+        <v>260</v>
+      </c>
+      <c r="E795">
+        <v>15</v>
+      </c>
+      <c r="F795" t="s">
+        <v>256</v>
+      </c>
+      <c r="G795">
+        <v>1</v>
+      </c>
+      <c r="H795">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="796" spans="1:8">
+      <c r="A796" s="5" t="s">
+        <v>1920</v>
+      </c>
+      <c r="B796" t="s">
+        <v>917</v>
+      </c>
+      <c r="C796" t="s">
+        <v>139</v>
+      </c>
+      <c r="D796" t="s">
+        <v>350</v>
+      </c>
+      <c r="E796">
+        <v>5</v>
+      </c>
+      <c r="F796" t="s">
+        <v>351</v>
+      </c>
+      <c r="G796">
+        <v>0</v>
+      </c>
+      <c r="H796">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="797" spans="1:8">
+      <c r="A797" s="5" t="s">
+        <v>1921</v>
+      </c>
+      <c r="B797" t="s">
+        <v>917</v>
+      </c>
+      <c r="C797" t="s">
+        <v>139</v>
+      </c>
+      <c r="D797" t="s">
+        <v>312</v>
+      </c>
+      <c r="E797">
+        <v>5</v>
+      </c>
+      <c r="G797">
+        <v>0</v>
+      </c>
+      <c r="H797">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H738" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}"/>
+  <autoFilter ref="A1:H774" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H525">
     <sortCondition ref="B2:B525"/>
     <sortCondition ref="C2:C525"/>
@@ -39879,8 +41519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B3BDA4-C76D-4F2B-A5C7-6A022A2D593F}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41115,11 +42755,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
-  <dimension ref="A1:C313"/>
+  <dimension ref="A1:C325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A297" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C312" sqref="C312"/>
+      <pane ySplit="1" topLeftCell="A309" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B332" sqref="B332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44572,6 +46212,138 @@
         <v>863</v>
       </c>
     </row>
+    <row r="314" spans="1:3">
+      <c r="A314" s="15" t="s">
+        <v>1892</v>
+      </c>
+      <c r="B314" s="8" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C314" s="8" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" s="15" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B315" s="8" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C315" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A316" s="15" t="s">
+        <v>1894</v>
+      </c>
+      <c r="B316" s="8" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C316" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" s="15" t="s">
+        <v>1895</v>
+      </c>
+      <c r="B317" s="8" t="s">
+        <v>1896</v>
+      </c>
+      <c r="C317" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" ht="30">
+      <c r="A318" t="s">
+        <v>1922</v>
+      </c>
+      <c r="B318" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C318" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" ht="30">
+      <c r="A319" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B319" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C319" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" ht="30">
+      <c r="A320" t="s">
+        <v>1924</v>
+      </c>
+      <c r="B320" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C320" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" ht="30">
+      <c r="A321" t="s">
+        <v>1925</v>
+      </c>
+      <c r="B321" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C321" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3" ht="30">
+      <c r="A322" t="s">
+        <v>1926</v>
+      </c>
+      <c r="B322" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C322" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3" ht="30">
+      <c r="A323" t="s">
+        <v>1927</v>
+      </c>
+      <c r="B323" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C323" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3" ht="30">
+      <c r="A324" t="s">
+        <v>1928</v>
+      </c>
+      <c r="B324" s="8" t="s">
+        <v>1930</v>
+      </c>
+      <c r="C324" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" t="s">
+        <v>1929</v>
+      </c>
+      <c r="B325" s="8" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C325" s="9" t="s">
+        <v>863</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C262" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -44580,10 +46352,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -44903,6 +46675,62 @@
         <v>1876</v>
       </c>
     </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>860</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>1898</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>917</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>1932</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>917</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>1933</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>1934</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>917</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>1931</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1935</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bugfixes and hobbit faction logos
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD373F90-33F3-4DD3-917D-B292C300AE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A77013D-DE3B-4783-BFDD-8542F1E4DD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">hero_constraints!$A$1:$C$263</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">models!$A$1:$J$626</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$G$825</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">options!$A$1:$G$1311</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9135" uniqueCount="2811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9141" uniqueCount="2813">
   <si>
     <t>faction</t>
   </si>
@@ -8611,6 +8611,12 @@
   </si>
   <si>
     <t>OPT1310</t>
+  </si>
+  <si>
+    <t>OPT1311</t>
+  </si>
+  <si>
+    <t>OPT1312</t>
   </si>
 </sst>
 </file>
@@ -31692,11 +31698,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
-  <dimension ref="A1:G1311"/>
+  <dimension ref="A1:G1313"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1301" sqref="D1301"/>
+      <pane ySplit="1" topLeftCell="A1286" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1301" sqref="B1301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -59929,8 +59935,50 @@
         <v>1</v>
       </c>
     </row>
+    <row r="1312" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1312" s="9" t="s">
+        <v>2811</v>
+      </c>
+      <c r="B1312" s="5" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1312" s="6" t="s">
+        <v>2254</v>
+      </c>
+      <c r="D1312" s="6">
+        <v>5</v>
+      </c>
+      <c r="E1312" s="6"/>
+      <c r="F1312" s="6">
+        <v>0</v>
+      </c>
+      <c r="G1312" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1313" s="9" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B1313" s="5" t="s">
+        <v>2322</v>
+      </c>
+      <c r="C1313" s="6" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D1313" s="6">
+        <v>5</v>
+      </c>
+      <c r="E1313" s="6"/>
+      <c r="F1313" s="6">
+        <v>0</v>
+      </c>
+      <c r="G1313" s="6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G825" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}"/>
+  <autoFilter ref="A1:G1311" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1305">
     <sortCondition ref="B2:B1305"/>
     <sortCondition descending="1" ref="D2:D1305"/>

</xml_diff>

<commit_message>
bugfix for warrior profile cards
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBDFA61-A05B-401B-8315-5712B3962925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC9659F-6906-411D-AEC3-B54F65F7FEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -9447,9 +9447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
   <dimension ref="A1:K652"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A456" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E466" sqref="E466"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A630" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D639" sqref="D639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32944,7 +32944,7 @@
   <dimension ref="A1:G1358"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A339" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1340" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B354" sqref="B354"/>
     </sheetView>
   </sheetViews>
@@ -62213,8 +62213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
   <dimension ref="A1:D442"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B139" sqref="B139"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Herald of the dead fix
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C016E766-8FA7-41AC-B730-2A0169126A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300AA259-02A3-449F-A7CA-92D3DFA88CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10679" uniqueCount="3138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10682" uniqueCount="3139">
   <si>
     <t>faction</t>
   </si>
@@ -9594,6 +9594,9 @@
   </si>
   <si>
     <t>exclusive</t>
+  </si>
+  <si>
+    <t>OPT1447</t>
   </si>
 </sst>
 </file>
@@ -35673,11 +35676,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
-  <dimension ref="A1:G1447"/>
+  <dimension ref="A1:G1448"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A481" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E494" sqref="E494"/>
+      <pane ySplit="1" topLeftCell="A1437" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1449" sqref="A1449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -66734,6 +66737,27 @@
         <v>0</v>
       </c>
       <c r="G1447" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1448" s="9" t="s">
+        <v>3138</v>
+      </c>
+      <c r="B1448" s="6" t="s">
+        <v>984</v>
+      </c>
+      <c r="C1448" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D1448" s="6">
+        <v>5</v>
+      </c>
+      <c r="E1448" s="6"/>
+      <c r="F1448" s="6">
+        <v>0</v>
+      </c>
+      <c r="G1448" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bill the pony fix
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9926E1D-9F6E-42DE-82D9-6F42898A770C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E16CF0-059B-432B-B8AA-654C0C24C544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12952" uniqueCount="3700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12956" uniqueCount="3701">
   <si>
     <t>faction</t>
   </si>
@@ -11293,6 +11293,9 @@
   </si>
   <si>
     <t>["Minas Tirith", "[minas_tirith] cirion"]</t>
+  </si>
+  <si>
+    <t>[wanderers_in_the_wild_(good)] bill_the_pony</t>
   </si>
 </sst>
 </file>
@@ -11829,8 +11832,8 @@
   <dimension ref="A1:K894"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A212" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A224" sqref="A224"/>
+      <pane ySplit="1" topLeftCell="A870" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A888" sqref="A888"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -80628,11 +80631,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}">
-  <dimension ref="A1:E616"/>
+  <dimension ref="A1:E617"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A603" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A617" sqref="A617"/>
+      <selection pane="bottomLeft" activeCell="B617" sqref="B617:E617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -89722,6 +89725,20 @@
         <v>846</v>
       </c>
     </row>
+    <row r="617" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A617" t="s">
+        <v>3700</v>
+      </c>
+      <c r="B617" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="C617" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="E617" t="s">
+        <v>846</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E511" xr:uid="{59CB009E-54DD-49E7-AF48-1368091BE4E1}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -89732,7 +89749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Black numenorean marshall fix
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29320E5-9908-49B2-9F67-A25B0D24A701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF50A50B-1182-4082-809E-DCC72039ECDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -44034,8 +44034,8 @@
   <dimension ref="A1:G1648"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1633" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1645" sqref="B1645"/>
+      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -45826,7 +45826,7 @@
         <v>257</v>
       </c>
       <c r="D83" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>253</v>
@@ -47767,7 +47767,7 @@
         <v>257</v>
       </c>
       <c r="D174" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E174" s="6" t="s">
         <v>253</v>
@@ -55793,7 +55793,7 @@
         <v>257</v>
       </c>
       <c r="D548" s="6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E548" s="6" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
Cave drakes are not unique
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9C8274-9768-4412-BA53-E232BEE58F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D43A2F-A71C-4DE9-9EFF-D48D8D04E1E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -11831,9 +11831,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
   <dimension ref="A1:K894"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E290" sqref="E290"/>
+      <selection pane="bottomLeft" activeCell="E304" sqref="E304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -22783,7 +22783,7 @@
         <v>0</v>
       </c>
       <c r="I304" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J304" s="6">
         <v>0</v>
@@ -44027,7 +44027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:G1644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
@@ -80322,7 +80322,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="325" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="338" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
         <v>947</v>
       </c>

</xml_diff>

<commit_message>
Assault on Lothlorien bonuses
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693AA7B9-8FFC-4264-88FC-39B7EC7FA3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE9BC8E-0468-468A-BEC9-2D7DF486CDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -10467,16 +10467,6 @@
     <t>[rangers_of_mirkwood] wood_elf_sentinel</t>
   </si>
   <si>
-    <t>An Assault on Lothlórien force must always include Muzgúr and at least one named Goblin Hero model. Muzgúr must always be the army’s leader.
-Only Orc Hero models may lead Orc Warrior models. Only Goblin Hero models may lead Goblin Warrior models.
-Spider models may only be included in warbands led by Drûzhag or Ashrâk.
-In this Legendary Legion, Muzgúr, Drûzhag and Ashrâk are Heroes of Valour, and Shamans are Heroes of Fortitude.
-&lt;b&gt;"Cover of Darkness"&lt;/b&gt; - Any battle featuring this Legendary Legion takes place at night. As such, due to the reduced visibility, models cannot be targeted by shooting, Magical Powers or special abilities over 12" away. However, as it is much harder to avoid a shot in the dark, all shooting attacks gain a bonus of +1 when rolling To Wound. Siege Engines may still target enemy models more than 12" away, however in this situation they will only ever hit on the roll of a 6. Models with the Cave Dweller special rule can see as normal.
-&lt;b&gt;"Ruthless Savagery"&lt;/b&gt; - Friendly Orc and Goblin models gain a bonus of +1 To Wound in a fight in which the opposing model is outnumbered. Note that supporting models do not count for either side for the purpose of this rule.
-&lt;b&gt;"Dark Magics"&lt;/b&gt; - Friendly models may re-roll any number of D6 when making a Casting roll.
-&lt;b&gt;"Venom-back Spiders"&lt;/b&gt; - If your force contains Ashrâk then all Giant Spiders in your force can be upgraded to Venom-back Spiders for free.</t>
-  </si>
-  <si>
     <t>A Defenders of Erebor force must always contain at least one named Erebor Hero model, and at least one named Dale Hero model.
 Only Erebor Hero models may lead Erebor Warrior models.
 Only Dale Hero models may lead Dale Warrior models.
@@ -11293,6 +11283,16 @@
   </si>
   <si>
     <t>['Halls of Thranduil', 'Lothlorien', 'The Misty Mountains', 'Tom Bombadil', 'Goldberry']</t>
+  </si>
+  <si>
+    <t>An Assault on Lothlórien force must always include Muzgúr and at least one named Goblin Hero model. Muzgúr must always be the army’s leader. This Legendary Legion may not include more Goblin models than Orc models
+Only Orc Hero models may lead Orc Warrior models. Only Goblin Hero models may lead Goblin Warrior models.
+Spider models may only be included in warbands led by Drûzhag or Ashrâk.
+In this Legendary Legion, Muzgúr, Drûzhag and Ashrâk are Heroes of Valour, and Shamans are Heroes of Fortitude.
+&lt;b&gt;"Cover of Darkness"&lt;/b&gt; - Any battle featuring this Legendary Legion takes place at night. As such, due to the reduced visibility, models cannot be targeted by shooting, Magical Powers or special abilities over 12" away. However, as it is much harder to avoid a shot in the dark, all shooting attacks gain a bonus of +1 when rolling To Wound. Siege Engines may still target enemy models more than 12" away, however in this situation they will only ever hit on the roll of a 6. Models with the Cave Dweller special rule can see as normal.
+&lt;b&gt;"Ruthless Savagery"&lt;/b&gt; - Friendly Orc and Goblin models gain a bonus of +1 To Wound in a fight in which the opposing model is outnumbered. Note that supporting models do not count for either side for the purpose of this rule.
+&lt;b&gt;"Dark Magics"&lt;/b&gt; - Friendly models may re-roll any number of D6 when making a Casting roll.
+&lt;b&gt;"Venom-back Spiders"&lt;/b&gt; - If your force contains Ashrâk then all Giant Spiders in your force can be upgraded to Venom-back Spiders for free.</t>
   </si>
 </sst>
 </file>
@@ -42214,7 +42214,7 @@
     </row>
     <row r="845" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A845" s="7" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="B845" s="6" t="s">
         <v>210</v>
@@ -42249,7 +42249,7 @@
     </row>
     <row r="846" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A846" s="7" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="B846" s="6" t="s">
         <v>210</v>
@@ -42392,7 +42392,7 @@
     </row>
     <row r="850" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A850" s="7" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="B850" s="6" t="s">
         <v>210</v>
@@ -42427,7 +42427,7 @@
     </row>
     <row r="851" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A851" s="7" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="B851" s="6" t="s">
         <v>210</v>
@@ -43657,13 +43657,13 @@
         <v>202</v>
       </c>
       <c r="C885" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D885" s="6" t="s">
         <v>959</v>
       </c>
       <c r="E885" s="6" t="s">
-        <v>3621</v>
+        <v>3620</v>
       </c>
       <c r="F885" s="6" t="s">
         <v>44</v>
@@ -43693,13 +43693,13 @@
         <v>202</v>
       </c>
       <c r="C886" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D886" s="6" t="s">
         <v>959</v>
       </c>
       <c r="E886" s="6" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="F886" s="6" t="s">
         <v>44</v>
@@ -43729,13 +43729,13 @@
         <v>202</v>
       </c>
       <c r="C887" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D887" s="6" t="s">
         <v>959</v>
       </c>
       <c r="E887" s="6" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="F887" s="6" t="s">
         <v>22</v>
@@ -43765,7 +43765,7 @@
         <v>202</v>
       </c>
       <c r="C888" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D888" s="6" t="s">
         <v>3</v>
@@ -43801,7 +43801,7 @@
         <v>202</v>
       </c>
       <c r="C889" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D889" s="6" t="s">
         <v>959</v>
@@ -43837,7 +43837,7 @@
         <v>202</v>
       </c>
       <c r="C890" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D890" s="6" t="s">
         <v>959</v>
@@ -43873,7 +43873,7 @@
         <v>202</v>
       </c>
       <c r="C891" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D891" s="6" t="s">
         <v>959</v>
@@ -43909,7 +43909,7 @@
         <v>202</v>
       </c>
       <c r="C892" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D892" s="6" t="s">
         <v>959</v>
@@ -43945,13 +43945,13 @@
         <v>202</v>
       </c>
       <c r="C893" s="6" t="s">
-        <v>3661</v>
+        <v>3660</v>
       </c>
       <c r="D893" s="6" t="s">
         <v>959</v>
       </c>
       <c r="E893" s="6" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="F893" s="6" t="s">
         <v>44</v>
@@ -43981,13 +43981,13 @@
         <v>203</v>
       </c>
       <c r="C894" s="6" t="s">
-        <v>3662</v>
+        <v>3661</v>
       </c>
       <c r="D894" s="6" t="s">
         <v>959</v>
       </c>
       <c r="E894" s="6" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="F894" s="6" t="s">
         <v>44</v>
@@ -73472,7 +73472,7 @@
         <v>1</v>
       </c>
       <c r="E1368" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="F1368" s="6">
         <v>0</v>
@@ -73515,7 +73515,7 @@
         <v>0</v>
       </c>
       <c r="E1370" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="F1370" s="6">
         <v>0</v>
@@ -74101,7 +74101,7 @@
         <v>1</v>
       </c>
       <c r="E1399" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="F1399" s="6">
         <v>0</v>
@@ -74144,7 +74144,7 @@
         <v>0</v>
       </c>
       <c r="E1401" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="F1401" s="6">
         <v>0</v>
@@ -74327,7 +74327,7 @@
         <v>1</v>
       </c>
       <c r="E1410" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="F1410" s="6">
         <v>0</v>
@@ -74370,7 +74370,7 @@
         <v>0</v>
       </c>
       <c r="E1412" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="F1412" s="6">
         <v>0</v>
@@ -77322,10 +77322,10 @@
     </row>
     <row r="1557" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1557" s="9" t="s">
-        <v>3442</v>
+        <v>3441</v>
       </c>
       <c r="B1557" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="C1557" s="6" t="s">
         <v>3034</v>
@@ -77342,10 +77342,10 @@
     </row>
     <row r="1558" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1558" s="9" t="s">
-        <v>3443</v>
+        <v>3442</v>
       </c>
       <c r="B1558" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="C1558" s="6" t="s">
         <v>309</v>
@@ -77362,10 +77362,10 @@
     </row>
     <row r="1559" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1559" s="9" t="s">
-        <v>3444</v>
+        <v>3443</v>
       </c>
       <c r="B1559" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="C1559" s="6" t="s">
         <v>2306</v>
@@ -77382,10 +77382,10 @@
     </row>
     <row r="1560" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1560" s="9" t="s">
-        <v>3445</v>
+        <v>3444</v>
       </c>
       <c r="B1560" t="s">
-        <v>3462</v>
+        <v>3461</v>
       </c>
       <c r="C1560" s="6" t="s">
         <v>2306</v>
@@ -77402,10 +77402,10 @@
     </row>
     <row r="1561" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1561" s="9" t="s">
-        <v>3446</v>
+        <v>3445</v>
       </c>
       <c r="B1561" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1561" s="6" t="s">
         <v>281</v>
@@ -77422,10 +77422,10 @@
     </row>
     <row r="1562" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1562" s="9" t="s">
-        <v>3447</v>
+        <v>3446</v>
       </c>
       <c r="B1562" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1562" s="6" t="s">
         <v>283</v>
@@ -77442,10 +77442,10 @@
     </row>
     <row r="1563" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1563" s="9" t="s">
-        <v>3448</v>
+        <v>3447</v>
       </c>
       <c r="B1563" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1563" s="6" t="s">
         <v>3034</v>
@@ -77465,10 +77465,10 @@
     </row>
     <row r="1564" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1564" s="9" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="B1564" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1564" s="6" t="s">
         <v>309</v>
@@ -77485,10 +77485,10 @@
     </row>
     <row r="1565" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1565" s="9" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="B1565" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1565" s="6" t="s">
         <v>317</v>
@@ -77505,10 +77505,10 @@
     </row>
     <row r="1566" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1566" s="9" t="s">
-        <v>3451</v>
+        <v>3450</v>
       </c>
       <c r="B1566" t="s">
-        <v>3463</v>
+        <v>3462</v>
       </c>
       <c r="C1566" s="6" t="s">
         <v>2306</v>
@@ -77525,10 +77525,10 @@
     </row>
     <row r="1567" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1567" s="9" t="s">
-        <v>3452</v>
+        <v>3451</v>
       </c>
       <c r="B1567" s="7" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
       <c r="C1567" s="6" t="s">
         <v>2890</v>
@@ -77545,10 +77545,10 @@
     </row>
     <row r="1568" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1568" s="9" t="s">
-        <v>3453</v>
+        <v>3452</v>
       </c>
       <c r="B1568" s="7" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
       <c r="C1568" s="6" t="s">
         <v>2306</v>
@@ -77565,10 +77565,10 @@
     </row>
     <row r="1569" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1569" s="9" t="s">
-        <v>3454</v>
+        <v>3453</v>
       </c>
       <c r="B1569" s="7" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
       <c r="C1569" s="6" t="s">
         <v>2888</v>
@@ -77585,10 +77585,10 @@
     </row>
     <row r="1570" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1570" s="9" t="s">
-        <v>3455</v>
+        <v>3454</v>
       </c>
       <c r="B1570" s="7" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="C1570" s="6" t="s">
         <v>283</v>
@@ -77605,10 +77605,10 @@
     </row>
     <row r="1571" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1571" s="9" t="s">
-        <v>3456</v>
+        <v>3455</v>
       </c>
       <c r="B1571" s="7" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="C1571" s="6" t="s">
         <v>317</v>
@@ -77625,10 +77625,10 @@
     </row>
     <row r="1572" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1572" s="9" t="s">
-        <v>3457</v>
+        <v>3456</v>
       </c>
       <c r="B1572" s="7" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="C1572" s="6" t="s">
         <v>2896</v>
@@ -77637,7 +77637,7 @@
         <v>1</v>
       </c>
       <c r="E1572" t="s">
-        <v>3695</v>
+        <v>3694</v>
       </c>
       <c r="F1572" s="6">
         <v>0</v>
@@ -77648,10 +77648,10 @@
     </row>
     <row r="1573" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1573" s="9" t="s">
-        <v>3458</v>
+        <v>3457</v>
       </c>
       <c r="B1573" s="7" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="C1573" s="6" t="s">
         <v>2306</v>
@@ -77668,10 +77668,10 @@
     </row>
     <row r="1574" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1574" s="9" t="s">
-        <v>3459</v>
+        <v>3458</v>
       </c>
       <c r="B1574" s="7" t="s">
-        <v>3465</v>
+        <v>3464</v>
       </c>
       <c r="C1574" s="6" t="s">
         <v>2897</v>
@@ -77680,7 +77680,7 @@
         <v>0</v>
       </c>
       <c r="E1574" t="s">
-        <v>3696</v>
+        <v>3695</v>
       </c>
       <c r="F1574" s="6">
         <v>0</v>
@@ -77691,10 +77691,10 @@
     </row>
     <row r="1575" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1575" s="9" t="s">
-        <v>3460</v>
+        <v>3459</v>
       </c>
       <c r="B1575" s="7" t="s">
-        <v>3466</v>
+        <v>3465</v>
       </c>
       <c r="C1575" s="6" t="s">
         <v>2306</v>
@@ -77711,10 +77711,10 @@
     </row>
     <row r="1576" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1576" s="9" t="s">
-        <v>3481</v>
+        <v>3480</v>
       </c>
       <c r="B1576" s="7" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="C1576" s="6" t="s">
         <v>3186</v>
@@ -77731,10 +77731,10 @@
     </row>
     <row r="1577" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1577" s="9" t="s">
-        <v>3482</v>
+        <v>3481</v>
       </c>
       <c r="B1577" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="C1577" s="6" t="s">
         <v>309</v>
@@ -77751,10 +77751,10 @@
     </row>
     <row r="1578" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1578" s="9" t="s">
-        <v>3483</v>
+        <v>3482</v>
       </c>
       <c r="B1578" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="C1578" s="6" t="s">
         <v>2306</v>
@@ -77771,10 +77771,10 @@
     </row>
     <row r="1579" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1579" s="9" t="s">
-        <v>3484</v>
+        <v>3483</v>
       </c>
       <c r="B1579" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="C1579" s="6" t="s">
         <v>283</v>
@@ -77791,10 +77791,10 @@
     </row>
     <row r="1580" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1580" s="9" t="s">
-        <v>3485</v>
+        <v>3484</v>
       </c>
       <c r="B1580" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="C1580" s="6" t="s">
         <v>309</v>
@@ -77811,10 +77811,10 @@
     </row>
     <row r="1581" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1581" s="9" t="s">
-        <v>3486</v>
+        <v>3485</v>
       </c>
       <c r="B1581" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="C1581" s="6" t="s">
         <v>317</v>
@@ -77831,10 +77831,10 @@
     </row>
     <row r="1582" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1582" s="9" t="s">
-        <v>3487</v>
+        <v>3486</v>
       </c>
       <c r="B1582" t="s">
-        <v>3500</v>
+        <v>3499</v>
       </c>
       <c r="C1582" s="6" t="s">
         <v>2306</v>
@@ -77851,10 +77851,10 @@
     </row>
     <row r="1583" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1583" s="9" t="s">
-        <v>3488</v>
+        <v>3487</v>
       </c>
       <c r="B1583" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="C1583" s="6" t="s">
         <v>2051</v>
@@ -77871,10 +77871,10 @@
     </row>
     <row r="1584" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1584" s="9" t="s">
-        <v>3489</v>
+        <v>3488</v>
       </c>
       <c r="B1584" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="C1584" s="6" t="s">
         <v>307</v>
@@ -77891,10 +77891,10 @@
     </row>
     <row r="1585" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1585" s="9" t="s">
-        <v>3490</v>
+        <v>3489</v>
       </c>
       <c r="B1585" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="C1585" s="6" t="s">
         <v>3197</v>
@@ -77911,10 +77911,10 @@
     </row>
     <row r="1586" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1586" s="9" t="s">
-        <v>3491</v>
+        <v>3490</v>
       </c>
       <c r="B1586" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="C1586" s="6" t="s">
         <v>2306</v>
@@ -77931,10 +77931,10 @@
     </row>
     <row r="1587" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1587" s="9" t="s">
-        <v>3492</v>
+        <v>3491</v>
       </c>
       <c r="B1587" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1587" s="6" t="s">
         <v>281</v>
@@ -77951,10 +77951,10 @@
     </row>
     <row r="1588" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1588" s="9" t="s">
-        <v>3493</v>
+        <v>3492</v>
       </c>
       <c r="B1588" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1588" s="6" t="s">
         <v>283</v>
@@ -77971,10 +77971,10 @@
     </row>
     <row r="1589" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1589" s="9" t="s">
-        <v>3494</v>
+        <v>3493</v>
       </c>
       <c r="B1589" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1589" s="6" t="s">
         <v>2051</v>
@@ -77991,10 +77991,10 @@
     </row>
     <row r="1590" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1590" s="9" t="s">
-        <v>3495</v>
+        <v>3494</v>
       </c>
       <c r="B1590" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1590" s="6" t="s">
         <v>307</v>
@@ -78014,10 +78014,10 @@
     </row>
     <row r="1591" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1591" s="9" t="s">
-        <v>3496</v>
+        <v>3495</v>
       </c>
       <c r="B1591" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1591" s="6" t="s">
         <v>3197</v>
@@ -78034,10 +78034,10 @@
     </row>
     <row r="1592" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1592" s="9" t="s">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="B1592" t="s">
-        <v>3502</v>
+        <v>3501</v>
       </c>
       <c r="C1592" s="6" t="s">
         <v>2306</v>
@@ -78054,7 +78054,7 @@
     </row>
     <row r="1593" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1593" s="9" t="s">
-        <v>3515</v>
+        <v>3514</v>
       </c>
       <c r="B1593" t="s">
         <v>3310</v>
@@ -78074,10 +78074,10 @@
     </row>
     <row r="1594" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1594" s="9" t="s">
-        <v>3516</v>
+        <v>3515</v>
       </c>
       <c r="B1594" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="C1594" s="6" t="s">
         <v>271</v>
@@ -78094,10 +78094,10 @@
     </row>
     <row r="1595" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1595" s="9" t="s">
+        <v>3516</v>
+      </c>
+      <c r="B1595" t="s">
         <v>3517</v>
-      </c>
-      <c r="B1595" t="s">
-        <v>3518</v>
       </c>
       <c r="C1595" s="6" t="s">
         <v>2306</v>
@@ -78114,10 +78114,10 @@
     </row>
     <row r="1596" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1596" s="9" t="s">
-        <v>3537</v>
+        <v>3536</v>
       </c>
       <c r="B1596" s="6" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="C1596" s="6" t="s">
         <v>305</v>
@@ -78137,10 +78137,10 @@
     </row>
     <row r="1597" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1597" s="9" t="s">
-        <v>3538</v>
+        <v>3537</v>
       </c>
       <c r="B1597" s="6" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="C1597" s="6" t="s">
         <v>307</v>
@@ -78158,10 +78158,10 @@
     </row>
     <row r="1598" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1598" s="9" t="s">
-        <v>3539</v>
+        <v>3538</v>
       </c>
       <c r="B1598" s="6" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="C1598" s="6" t="s">
         <v>309</v>
@@ -78179,10 +78179,10 @@
     </row>
     <row r="1599" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1599" s="9" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="B1599" s="6" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="C1599" s="6" t="s">
         <v>2306</v>
@@ -78200,10 +78200,10 @@
     </row>
     <row r="1600" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1600" s="9" t="s">
-        <v>3541</v>
+        <v>3540</v>
       </c>
       <c r="B1600" s="6" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="C1600" s="6" t="s">
         <v>2306</v>
@@ -78221,10 +78221,10 @@
     </row>
     <row r="1601" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1601" s="9" t="s">
-        <v>3542</v>
+        <v>3541</v>
       </c>
       <c r="B1601" s="6" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="C1601" s="6" t="s">
         <v>305</v>
@@ -78244,10 +78244,10 @@
     </row>
     <row r="1602" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1602" s="9" t="s">
-        <v>3543</v>
+        <v>3542</v>
       </c>
       <c r="B1602" s="6" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="C1602" s="6" t="s">
         <v>2306</v>
@@ -78265,10 +78265,10 @@
     </row>
     <row r="1603" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1603" s="9" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="B1603" s="6" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="C1603" s="6" t="s">
         <v>2306</v>
@@ -78286,10 +78286,10 @@
     </row>
     <row r="1604" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1604" s="9" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="B1604" s="6" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="C1604" s="6" t="s">
         <v>305</v>
@@ -78309,10 +78309,10 @@
     </row>
     <row r="1605" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1605" s="9" t="s">
-        <v>3546</v>
+        <v>3545</v>
       </c>
       <c r="B1605" s="5" t="s">
-        <v>3534</v>
+        <v>3533</v>
       </c>
       <c r="C1605" s="6" t="s">
         <v>2306</v>
@@ -78330,10 +78330,10 @@
     </row>
     <row r="1606" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1606" s="9" t="s">
-        <v>3547</v>
+        <v>3546</v>
       </c>
       <c r="B1606" s="6" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1606" s="6" t="s">
         <v>283</v>
@@ -78351,10 +78351,10 @@
     </row>
     <row r="1607" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1607" s="9" t="s">
-        <v>3548</v>
+        <v>3547</v>
       </c>
       <c r="B1607" s="6" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1607" s="6" t="s">
         <v>307</v>
@@ -78374,10 +78374,10 @@
     </row>
     <row r="1608" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1608" s="9" t="s">
-        <v>3549</v>
+        <v>3548</v>
       </c>
       <c r="B1608" s="6" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1608" s="6" t="s">
         <v>309</v>
@@ -78395,10 +78395,10 @@
     </row>
     <row r="1609" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1609" s="9" t="s">
-        <v>3550</v>
+        <v>3549</v>
       </c>
       <c r="B1609" s="6" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1609" s="6" t="s">
         <v>317</v>
@@ -78416,10 +78416,10 @@
     </row>
     <row r="1610" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1610" s="9" t="s">
-        <v>3551</v>
+        <v>3550</v>
       </c>
       <c r="B1610" s="6" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1610" s="6" t="s">
         <v>288</v>
@@ -78437,10 +78437,10 @@
     </row>
     <row r="1611" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1611" s="9" t="s">
-        <v>3552</v>
+        <v>3551</v>
       </c>
       <c r="B1611" s="5" t="s">
-        <v>3535</v>
+        <v>3534</v>
       </c>
       <c r="C1611" s="6" t="s">
         <v>2306</v>
@@ -78458,10 +78458,10 @@
     </row>
     <row r="1612" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1612" s="9" t="s">
-        <v>3553</v>
+        <v>3552</v>
       </c>
       <c r="B1612" s="6" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C1612" s="6" t="s">
         <v>283</v>
@@ -78479,10 +78479,10 @@
     </row>
     <row r="1613" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1613" s="9" t="s">
-        <v>3554</v>
+        <v>3553</v>
       </c>
       <c r="B1613" s="6" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C1613" s="6" t="s">
         <v>307</v>
@@ -78502,10 +78502,10 @@
     </row>
     <row r="1614" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1614" s="9" t="s">
-        <v>3555</v>
+        <v>3554</v>
       </c>
       <c r="B1614" s="6" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C1614" s="6" t="s">
         <v>309</v>
@@ -78523,10 +78523,10 @@
     </row>
     <row r="1615" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1615" s="9" t="s">
-        <v>3556</v>
+        <v>3555</v>
       </c>
       <c r="B1615" s="6" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C1615" s="6" t="s">
         <v>328</v>
@@ -78544,10 +78544,10 @@
     </row>
     <row r="1616" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1616" s="9" t="s">
-        <v>3557</v>
+        <v>3556</v>
       </c>
       <c r="B1616" s="5" t="s">
-        <v>3536</v>
+        <v>3535</v>
       </c>
       <c r="C1616" s="6" t="s">
         <v>2306</v>
@@ -78565,10 +78565,10 @@
     </row>
     <row r="1617" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1617" s="9" t="s">
-        <v>3584</v>
+        <v>3583</v>
       </c>
       <c r="B1617" s="6" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C1617" s="6" t="s">
         <v>305</v>
@@ -78588,10 +78588,10 @@
     </row>
     <row r="1618" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1618" s="9" t="s">
-        <v>3585</v>
+        <v>3584</v>
       </c>
       <c r="B1618" s="6" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C1618" s="6" t="s">
         <v>307</v>
@@ -78609,10 +78609,10 @@
     </row>
     <row r="1619" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1619" s="9" t="s">
-        <v>3586</v>
+        <v>3585</v>
       </c>
       <c r="B1619" s="6" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C1619" s="6" t="s">
         <v>309</v>
@@ -78630,10 +78630,10 @@
     </row>
     <row r="1620" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1620" s="9" t="s">
-        <v>3587</v>
+        <v>3586</v>
       </c>
       <c r="B1620" s="6" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="C1620" s="6" t="s">
         <v>2306</v>
@@ -78651,10 +78651,10 @@
     </row>
     <row r="1621" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1621" s="9" t="s">
-        <v>3588</v>
+        <v>3587</v>
       </c>
       <c r="B1621" s="6" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C1621" s="6" t="s">
         <v>305</v>
@@ -78674,10 +78674,10 @@
     </row>
     <row r="1622" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1622" s="9" t="s">
-        <v>3589</v>
+        <v>3588</v>
       </c>
       <c r="B1622" s="6" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="C1622" s="6" t="s">
         <v>2306</v>
@@ -78695,10 +78695,10 @@
     </row>
     <row r="1623" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1623" s="9" t="s">
-        <v>3590</v>
+        <v>3589</v>
       </c>
       <c r="B1623" s="6" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="C1623" s="6" t="s">
         <v>305</v>
@@ -78718,10 +78718,10 @@
     </row>
     <row r="1624" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1624" s="9" t="s">
-        <v>3591</v>
+        <v>3590</v>
       </c>
       <c r="B1624" s="5" t="s">
-        <v>3578</v>
+        <v>3577</v>
       </c>
       <c r="C1624" s="6" t="s">
         <v>2306</v>
@@ -78739,10 +78739,10 @@
     </row>
     <row r="1625" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1625" s="9" t="s">
-        <v>3592</v>
+        <v>3591</v>
       </c>
       <c r="B1625" s="6" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1625" s="6" t="s">
         <v>283</v>
@@ -78760,10 +78760,10 @@
     </row>
     <row r="1626" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1626" s="9" t="s">
-        <v>3593</v>
+        <v>3592</v>
       </c>
       <c r="B1626" s="6" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1626" s="6" t="s">
         <v>307</v>
@@ -78783,10 +78783,10 @@
     </row>
     <row r="1627" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1627" s="9" t="s">
-        <v>3594</v>
+        <v>3593</v>
       </c>
       <c r="B1627" s="6" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1627" s="6" t="s">
         <v>309</v>
@@ -78804,10 +78804,10 @@
     </row>
     <row r="1628" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1628" s="9" t="s">
-        <v>3595</v>
+        <v>3594</v>
       </c>
       <c r="B1628" s="6" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1628" s="6" t="s">
         <v>317</v>
@@ -78825,10 +78825,10 @@
     </row>
     <row r="1629" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1629" s="9" t="s">
-        <v>3596</v>
+        <v>3595</v>
       </c>
       <c r="B1629" s="6" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1629" s="6" t="s">
         <v>288</v>
@@ -78846,10 +78846,10 @@
     </row>
     <row r="1630" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1630" s="9" t="s">
-        <v>3597</v>
+        <v>3596</v>
       </c>
       <c r="B1630" s="5" t="s">
-        <v>3579</v>
+        <v>3578</v>
       </c>
       <c r="C1630" s="6" t="s">
         <v>2306</v>
@@ -78867,10 +78867,10 @@
     </row>
     <row r="1631" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1631" s="9" t="s">
-        <v>3598</v>
+        <v>3597</v>
       </c>
       <c r="B1631" s="6" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C1631" s="6" t="s">
         <v>283</v>
@@ -78888,10 +78888,10 @@
     </row>
     <row r="1632" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1632" s="9" t="s">
-        <v>3599</v>
+        <v>3598</v>
       </c>
       <c r="B1632" s="6" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C1632" s="6" t="s">
         <v>307</v>
@@ -78911,10 +78911,10 @@
     </row>
     <row r="1633" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1633" s="9" t="s">
-        <v>3600</v>
+        <v>3599</v>
       </c>
       <c r="B1633" s="6" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C1633" s="6" t="s">
         <v>309</v>
@@ -78932,10 +78932,10 @@
     </row>
     <row r="1634" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1634" s="9" t="s">
-        <v>3601</v>
+        <v>3600</v>
       </c>
       <c r="B1634" s="6" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C1634" s="6" t="s">
         <v>328</v>
@@ -78953,10 +78953,10 @@
     </row>
     <row r="1635" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1635" s="9" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B1635" s="5" t="s">
-        <v>3580</v>
+        <v>3579</v>
       </c>
       <c r="C1635" s="6" t="s">
         <v>2306</v>
@@ -78974,10 +78974,10 @@
     </row>
     <row r="1636" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1636" s="9" t="s">
-        <v>3603</v>
+        <v>3602</v>
       </c>
       <c r="B1636" s="5" t="s">
-        <v>3582</v>
+        <v>3581</v>
       </c>
       <c r="C1636" s="6" t="s">
         <v>2306</v>
@@ -78995,10 +78995,10 @@
     </row>
     <row r="1637" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1637" s="9" t="s">
-        <v>3604</v>
+        <v>3603</v>
       </c>
       <c r="B1637" s="6" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C1637" s="6" t="s">
         <v>307</v>
@@ -79018,10 +79018,10 @@
     </row>
     <row r="1638" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1638" s="9" t="s">
-        <v>3605</v>
+        <v>3604</v>
       </c>
       <c r="B1638" s="6" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C1638" s="6" t="s">
         <v>309</v>
@@ -79039,10 +79039,10 @@
     </row>
     <row r="1639" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1639" s="9" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="B1639" s="6" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C1639" s="6" t="s">
         <v>317</v>
@@ -79060,10 +79060,10 @@
     </row>
     <row r="1640" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1640" s="9" t="s">
-        <v>3607</v>
+        <v>3606</v>
       </c>
       <c r="B1640" s="5" t="s">
-        <v>3583</v>
+        <v>3582</v>
       </c>
       <c r="C1640" s="6" t="s">
         <v>2306</v>
@@ -79081,10 +79081,10 @@
     </row>
     <row r="1641" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1641" s="9" t="s">
-        <v>3608</v>
+        <v>3607</v>
       </c>
       <c r="B1641" s="5" t="s">
-        <v>3581</v>
+        <v>3580</v>
       </c>
       <c r="C1641" s="6" t="s">
         <v>2306</v>
@@ -79102,10 +79102,10 @@
     </row>
     <row r="1642" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1642" s="9" t="s">
+        <v>3692</v>
+      </c>
+      <c r="B1642" t="s">
         <v>3693</v>
-      </c>
-      <c r="B1642" t="s">
-        <v>3694</v>
       </c>
       <c r="C1642" s="6" t="s">
         <v>3414</v>
@@ -79125,7 +79125,7 @@
     </row>
     <row r="1643" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1643" s="9" t="s">
-        <v>3698</v>
+        <v>3697</v>
       </c>
       <c r="B1643" s="6" t="s">
         <v>995</v>
@@ -79160,8 +79160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B3BDA4-C76D-4F2B-A5C7-6A022A2D593F}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -79201,7 +79201,7 @@
         <v>828</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
       <c r="E2" s="12">
         <v>0.33</v>
@@ -79235,7 +79235,7 @@
         <v>832</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="E4" s="12">
         <v>0.33</v>
@@ -79262,10 +79262,10 @@
         <v>833</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="E6" s="12">
         <v>0.33</v>
@@ -79282,7 +79282,7 @@
         <v>836</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="E7" s="12">
         <v>0.33</v>
@@ -79296,10 +79296,10 @@
         <v>837</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
       <c r="E8" s="12">
         <v>0.33</v>
@@ -79316,7 +79316,7 @@
         <v>3028</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>3623</v>
+        <v>3622</v>
       </c>
       <c r="E9" s="12">
         <v>0.33</v>
@@ -79376,7 +79376,7 @@
         <v>846</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>3624</v>
+        <v>3623</v>
       </c>
       <c r="E13" s="12">
         <v>0.33</v>
@@ -79449,7 +79449,7 @@
         <v>3065</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="E18" s="12">
         <v>0.33</v>
@@ -79466,7 +79466,7 @@
         <v>853</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="E19" s="12">
         <v>0.33</v>
@@ -79509,7 +79509,7 @@
         <v>856</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
       <c r="E22" s="12">
         <v>0.33</v>
@@ -79520,7 +79520,7 @@
         <v>242</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>3617</v>
+        <v>3616</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11"/>
@@ -79644,7 +79644,7 @@
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>3625</v>
+        <v>3624</v>
       </c>
       <c r="E31" s="12">
         <v>0.33</v>
@@ -79687,7 +79687,7 @@
         <v>241</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>3620</v>
+        <v>3619</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
@@ -79723,7 +79723,7 @@
         <v>1530</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="E36" s="12">
         <v>0.33</v>
@@ -79753,7 +79753,7 @@
         <v>3085</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
       <c r="E38" s="12">
         <v>0.33</v>
@@ -79770,7 +79770,7 @@
         <v>882</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="E39" s="12">
         <v>0.33</v>
@@ -79787,7 +79787,7 @@
         <v>884</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="E40" s="12">
         <v>0.33</v>
@@ -79811,7 +79811,7 @@
         <v>886</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>3441</v>
+        <v>3440</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
@@ -79843,7 +79843,7 @@
         <v>890</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>3699</v>
+        <v>3698</v>
       </c>
       <c r="E44" s="12">
         <v>0.33</v>
@@ -79873,7 +79873,7 @@
         <v>894</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="E46" s="12">
         <v>0.33</v>
@@ -79890,7 +79890,7 @@
         <v>842</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="E47" s="12">
         <v>0.33</v>
@@ -79907,7 +79907,7 @@
         <v>2999</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
       <c r="E48" s="12">
         <v>0.33</v>
@@ -79924,7 +79924,7 @@
         <v>901</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
       <c r="E49" s="12">
         <v>0.33</v>
@@ -79938,10 +79938,10 @@
         <v>902</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="E50" s="12">
         <v>0.33</v>
@@ -79992,7 +79992,7 @@
         <v>910</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="E53" s="12">
         <v>0.33</v>
@@ -80035,7 +80035,7 @@
         <v>914</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
       <c r="E56" s="12">
         <v>0.33</v>
@@ -80049,10 +80049,10 @@
         <v>3156</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>3659</v>
+        <v>3658</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="E57" s="12">
         <v>0.33</v>
@@ -80082,7 +80082,7 @@
         <v>918</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="E59" s="12">
         <v>0.33</v>
@@ -80106,7 +80106,7 @@
         <v>920</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>3697</v>
+        <v>3696</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11"/>
@@ -80153,7 +80153,7 @@
         <v>928</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>3480</v>
+        <v>3479</v>
       </c>
       <c r="C64" s="11"/>
       <c r="D64" s="11"/>
@@ -80185,7 +80185,7 @@
         <v>842</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
       <c r="E66" s="12">
         <v>0.33</v>
@@ -80199,7 +80199,7 @@
         <v>933</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>3660</v>
+        <v>3659</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>934</v>
@@ -80213,7 +80213,7 @@
         <v>935</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>3529</v>
+        <v>3528</v>
       </c>
       <c r="C68" s="11"/>
       <c r="D68" s="11"/>
@@ -80238,12 +80238,12 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="351" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="364" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
         <v>939</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>3440</v>
+        <v>3699</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11"/>
@@ -80262,7 +80262,7 @@
         <v>3175</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="E71" s="12">
         <v>0.33</v>
@@ -80329,7 +80329,7 @@
         <v>950</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="C76" s="11"/>
       <c r="D76" s="11"/>
@@ -80359,7 +80359,7 @@
         <v>953</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>3528</v>
+        <v>3527</v>
       </c>
       <c r="C78" s="11"/>
       <c r="D78" s="11"/>
@@ -80412,16 +80412,16 @@
     </row>
     <row r="82" spans="1:5" ht="143" x14ac:dyDescent="0.35">
       <c r="A82" s="25" t="s">
+        <v>3620</v>
+      </c>
+      <c r="B82" s="26" t="s">
+        <v>3681</v>
+      </c>
+      <c r="C82" s="27" t="s">
+        <v>3672</v>
+      </c>
+      <c r="D82" s="26" t="s">
         <v>3621</v>
-      </c>
-      <c r="B82" s="26" t="s">
-        <v>3682</v>
-      </c>
-      <c r="C82" s="27" t="s">
-        <v>3673</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>3622</v>
       </c>
       <c r="E82" s="12">
         <v>0.33</v>
@@ -80429,16 +80429,16 @@
     </row>
     <row r="83" spans="1:5" ht="143" x14ac:dyDescent="0.35">
       <c r="A83" s="25" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="C83" s="27" t="s">
-        <v>3674</v>
+        <v>3673</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>3622</v>
+        <v>3621</v>
       </c>
       <c r="E83" s="12">
         <v>0.33</v>
@@ -80446,16 +80446,16 @@
     </row>
     <row r="84" spans="1:5" ht="52" x14ac:dyDescent="0.35">
       <c r="A84" s="25" t="s">
+        <v>3630</v>
+      </c>
+      <c r="B84" s="26" t="s">
+        <v>3681</v>
+      </c>
+      <c r="C84" s="27" t="s">
+        <v>3674</v>
+      </c>
+      <c r="D84" s="26" t="s">
         <v>3631</v>
-      </c>
-      <c r="B84" s="26" t="s">
-        <v>3682</v>
-      </c>
-      <c r="C84" s="27" t="s">
-        <v>3675</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>3632</v>
       </c>
       <c r="E84" s="12">
         <v>0.33</v>
@@ -80466,13 +80466,13 @@
         <v>3411</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="C85" s="27" t="s">
-        <v>3676</v>
+        <v>3675</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>3681</v>
+        <v>3680</v>
       </c>
       <c r="E85" s="12">
         <v>0.33</v>
@@ -80483,13 +80483,13 @@
         <v>1449</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="C86" s="27" t="s">
-        <v>3678</v>
+        <v>3677</v>
       </c>
       <c r="D86" s="26" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="E86" s="12">
         <v>0.33</v>
@@ -80500,13 +80500,13 @@
         <v>2915</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="C87" s="27" t="s">
+        <v>3678</v>
+      </c>
+      <c r="D87" s="26" t="s">
         <v>3679</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>3680</v>
       </c>
       <c r="E87" s="12">
         <v>0.33</v>
@@ -80514,13 +80514,13 @@
     </row>
     <row r="88" spans="1:5" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A88" s="25" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>3682</v>
+        <v>3681</v>
       </c>
       <c r="C88" s="27" t="s">
-        <v>3677</v>
+        <v>3676</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>842</v>
@@ -80531,13 +80531,13 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="25" t="s">
+        <v>3656</v>
+      </c>
+      <c r="B89" s="26" t="s">
+        <v>3681</v>
+      </c>
+      <c r="C89" s="27" t="s">
         <v>3657</v>
-      </c>
-      <c r="B89" s="26" t="s">
-        <v>3682</v>
-      </c>
-      <c r="C89" s="27" t="s">
-        <v>3658</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>842</v>
@@ -88889,7 +88889,7 @@
         <v>842</v>
       </c>
       <c r="E562" t="s">
-        <v>3479</v>
+        <v>3478</v>
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.35">
@@ -88936,10 +88936,10 @@
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A566" t="s">
+        <v>3466</v>
+      </c>
+      <c r="B566" s="1" t="s">
         <v>3467</v>
-      </c>
-      <c r="B566" s="1" t="s">
-        <v>3468</v>
       </c>
       <c r="C566" s="1" t="s">
         <v>842</v>
@@ -88950,10 +88950,10 @@
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>3469</v>
+        <v>3468</v>
       </c>
       <c r="B567" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C567" s="1" t="s">
         <v>842</v>
@@ -88964,10 +88964,10 @@
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>3470</v>
+        <v>3469</v>
       </c>
       <c r="B568" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C568" s="1" t="s">
         <v>842</v>
@@ -88978,10 +88978,10 @@
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>3471</v>
+        <v>3470</v>
       </c>
       <c r="B569" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C569" s="1" t="s">
         <v>842</v>
@@ -88992,10 +88992,10 @@
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>3472</v>
+        <v>3471</v>
       </c>
       <c r="B570" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C570" s="1" t="s">
         <v>842</v>
@@ -89006,10 +89006,10 @@
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
-        <v>3473</v>
+        <v>3472</v>
       </c>
       <c r="B571" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C571" s="1" t="s">
         <v>842</v>
@@ -89020,10 +89020,10 @@
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A572" t="s">
-        <v>3464</v>
+        <v>3463</v>
       </c>
       <c r="B572" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C572" s="1" t="s">
         <v>842</v>
@@ -89034,10 +89034,10 @@
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A573" t="s">
-        <v>3474</v>
+        <v>3473</v>
       </c>
       <c r="B573" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C573" s="1" t="s">
         <v>842</v>
@@ -89048,10 +89048,10 @@
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
-        <v>3475</v>
+        <v>3474</v>
       </c>
       <c r="B574" s="1" t="s">
-        <v>3468</v>
+        <v>3467</v>
       </c>
       <c r="C574" s="1" t="s">
         <v>842</v>
@@ -89062,10 +89062,10 @@
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
+        <v>3475</v>
+      </c>
+      <c r="B575" s="1" t="s">
         <v>3476</v>
-      </c>
-      <c r="B575" s="1" t="s">
-        <v>3477</v>
       </c>
       <c r="C575" s="1" t="s">
         <v>842</v>
@@ -89076,10 +89076,10 @@
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
-        <v>3478</v>
+        <v>3477</v>
       </c>
       <c r="B576" s="1" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
       <c r="C576" s="1" t="s">
         <v>842</v>
@@ -89090,10 +89090,10 @@
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>3461</v>
+        <v>3460</v>
       </c>
       <c r="B577" s="1" t="s">
-        <v>3477</v>
+        <v>3476</v>
       </c>
       <c r="C577" s="1" t="s">
         <v>842</v>
@@ -89104,10 +89104,10 @@
     </row>
     <row r="578" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
-        <v>3498</v>
+        <v>3497</v>
       </c>
       <c r="B578" s="1" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="C578" s="1" t="s">
         <v>842</v>
@@ -89118,10 +89118,10 @@
     </row>
     <row r="579" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A579" t="s">
-        <v>3503</v>
+        <v>3502</v>
       </c>
       <c r="B579" s="1" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="C579" s="1" t="s">
         <v>842</v>
@@ -89132,10 +89132,10 @@
     </row>
     <row r="580" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A580" t="s">
-        <v>3499</v>
+        <v>3498</v>
       </c>
       <c r="B580" s="1" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="C580" s="1" t="s">
         <v>842</v>
@@ -89146,10 +89146,10 @@
     </row>
     <row r="581" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A581" t="s">
-        <v>3501</v>
+        <v>3500</v>
       </c>
       <c r="B581" s="1" t="s">
-        <v>3505</v>
+        <v>3504</v>
       </c>
       <c r="C581" s="1" t="s">
         <v>842</v>
@@ -89160,7 +89160,7 @@
     </row>
     <row r="582" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A582" t="s">
-        <v>3504</v>
+        <v>3503</v>
       </c>
       <c r="B582" s="1" t="s">
         <v>842</v>
@@ -89174,10 +89174,10 @@
     </row>
     <row r="583" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A583" t="s">
-        <v>3518</v>
+        <v>3517</v>
       </c>
       <c r="B583" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C583" s="1" t="s">
         <v>842</v>
@@ -89188,10 +89188,10 @@
     </row>
     <row r="584" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A584" t="s">
-        <v>3519</v>
+        <v>3518</v>
       </c>
       <c r="B584" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C584" s="1" t="s">
         <v>842</v>
@@ -89202,10 +89202,10 @@
     </row>
     <row r="585" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A585" t="s">
-        <v>3511</v>
+        <v>3510</v>
       </c>
       <c r="B585" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C585" s="1" t="s">
         <v>842</v>
@@ -89216,10 +89216,10 @@
     </row>
     <row r="586" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A586" t="s">
-        <v>3512</v>
+        <v>3511</v>
       </c>
       <c r="B586" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C586" s="1" t="s">
         <v>842</v>
@@ -89230,10 +89230,10 @@
     </row>
     <row r="587" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A587" t="s">
-        <v>3510</v>
+        <v>3509</v>
       </c>
       <c r="B587" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C587" s="1" t="s">
         <v>842</v>
@@ -89244,10 +89244,10 @@
     </row>
     <row r="588" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A588" t="s">
-        <v>3520</v>
+        <v>3519</v>
       </c>
       <c r="B588" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C588" s="1" t="s">
         <v>842</v>
@@ -89258,10 +89258,10 @@
     </row>
     <row r="589" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>3521</v>
+        <v>3520</v>
       </c>
       <c r="B589" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C589" s="1" t="s">
         <v>842</v>
@@ -89272,10 +89272,10 @@
     </row>
     <row r="590" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A590" t="s">
-        <v>3513</v>
+        <v>3512</v>
       </c>
       <c r="B590" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C590" s="1" t="s">
         <v>842</v>
@@ -89286,10 +89286,10 @@
     </row>
     <row r="591" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A591" t="s">
-        <v>3514</v>
+        <v>3513</v>
       </c>
       <c r="B591" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C591" s="1" t="s">
         <v>842</v>
@@ -89300,10 +89300,10 @@
     </row>
     <row r="592" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A592" t="s">
-        <v>3522</v>
+        <v>3521</v>
       </c>
       <c r="B592" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C592" s="1" t="s">
         <v>842</v>
@@ -89314,10 +89314,10 @@
     </row>
     <row r="593" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A593" t="s">
-        <v>3523</v>
+        <v>3522</v>
       </c>
       <c r="B593" s="1" t="s">
-        <v>3525</v>
+        <v>3524</v>
       </c>
       <c r="C593" s="1" t="s">
         <v>842</v>
@@ -89328,10 +89328,10 @@
     </row>
     <row r="594" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A594" t="s">
+        <v>3523</v>
+      </c>
+      <c r="B594" s="1" t="s">
         <v>3524</v>
-      </c>
-      <c r="B594" s="1" t="s">
-        <v>3525</v>
       </c>
       <c r="C594" s="1" t="s">
         <v>842</v>
@@ -89342,10 +89342,10 @@
     </row>
     <row r="595" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A595" t="s">
-        <v>3558</v>
+        <v>3557</v>
       </c>
       <c r="B595" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="C595" s="1" t="s">
         <v>842</v>
@@ -89356,10 +89356,10 @@
     </row>
     <row r="596" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A596" t="s">
-        <v>3530</v>
+        <v>3529</v>
       </c>
       <c r="B596" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="C596" s="1" t="s">
         <v>842</v>
@@ -89370,10 +89370,10 @@
     </row>
     <row r="597" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A597" t="s">
-        <v>3532</v>
+        <v>3531</v>
       </c>
       <c r="B597" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="C597" s="1" t="s">
         <v>842</v>
@@ -89384,10 +89384,10 @@
     </row>
     <row r="598" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A598" t="s">
-        <v>3533</v>
+        <v>3532</v>
       </c>
       <c r="B598" s="1" t="s">
-        <v>3560</v>
+        <v>3559</v>
       </c>
       <c r="C598" s="1" t="s">
         <v>842</v>
@@ -89398,7 +89398,7 @@
     </row>
     <row r="599" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A599" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="B599" s="1" t="s">
         <v>842</v>
@@ -89412,10 +89412,10 @@
     </row>
     <row r="600" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A600" t="s">
+        <v>3558</v>
+      </c>
+      <c r="B600" s="1" t="s">
         <v>3559</v>
-      </c>
-      <c r="B600" s="1" t="s">
-        <v>3560</v>
       </c>
       <c r="C600" s="1" t="s">
         <v>842</v>
@@ -89426,10 +89426,10 @@
     </row>
     <row r="601" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A601" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
       <c r="B601" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C601" s="1" t="s">
         <v>842</v>
@@ -89440,10 +89440,10 @@
     </row>
     <row r="602" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A602" t="s">
-        <v>3567</v>
+        <v>3566</v>
       </c>
       <c r="B602" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C602" s="1" t="s">
         <v>842</v>
@@ -89454,10 +89454,10 @@
     </row>
     <row r="603" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A603" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
       <c r="B603" s="1" t="s">
-        <v>3574</v>
+        <v>3573</v>
       </c>
       <c r="C603" s="1" t="s">
         <v>842</v>
@@ -89468,10 +89468,10 @@
     </row>
     <row r="604" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A604" t="s">
-        <v>3569</v>
+        <v>3568</v>
       </c>
       <c r="B604" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C604" s="1" t="s">
         <v>842</v>
@@ -89482,10 +89482,10 @@
     </row>
     <row r="605" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A605" t="s">
-        <v>3570</v>
+        <v>3569</v>
       </c>
       <c r="B605" s="1" t="s">
-        <v>3575</v>
+        <v>3574</v>
       </c>
       <c r="C605" s="1" t="s">
         <v>842</v>
@@ -89496,10 +89496,10 @@
     </row>
     <row r="606" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A606" t="s">
-        <v>3571</v>
+        <v>3570</v>
       </c>
       <c r="B606" s="1" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="C606" s="1" t="s">
         <v>842</v>
@@ -89510,10 +89510,10 @@
     </row>
     <row r="607" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A607" t="s">
-        <v>3572</v>
+        <v>3571</v>
       </c>
       <c r="B607" s="1" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
       <c r="C607" s="1" t="s">
         <v>842</v>
@@ -89524,10 +89524,10 @@
     </row>
     <row r="608" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A608" t="s">
-        <v>3573</v>
+        <v>3572</v>
       </c>
       <c r="B608" s="1" t="s">
-        <v>3577</v>
+        <v>3576</v>
       </c>
       <c r="C608" s="1" t="s">
         <v>842</v>
@@ -89538,7 +89538,7 @@
     </row>
     <row r="609" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A609" t="s">
-        <v>3663</v>
+        <v>3662</v>
       </c>
       <c r="B609" s="1" t="s">
         <v>842</v>
@@ -89552,7 +89552,7 @@
     </row>
     <row r="610" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A610" t="s">
-        <v>3664</v>
+        <v>3663</v>
       </c>
       <c r="B610" s="1" t="s">
         <v>842</v>
@@ -89566,10 +89566,10 @@
     </row>
     <row r="611" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A611" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="B611" s="1" t="s">
-        <v>3671</v>
+        <v>3670</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>842</v>
@@ -89580,10 +89580,10 @@
     </row>
     <row r="612" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A612" t="s">
-        <v>3666</v>
+        <v>3665</v>
       </c>
       <c r="B612" s="1" t="s">
-        <v>3672</v>
+        <v>3671</v>
       </c>
       <c r="C612" s="1" t="s">
         <v>842</v>
@@ -89594,7 +89594,7 @@
     </row>
     <row r="613" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A613" t="s">
-        <v>3667</v>
+        <v>3666</v>
       </c>
       <c r="B613" s="1" t="s">
         <v>842</v>
@@ -89608,7 +89608,7 @@
     </row>
     <row r="614" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A614" t="s">
-        <v>3668</v>
+        <v>3667</v>
       </c>
       <c r="B614" s="1" t="s">
         <v>842</v>
@@ -89622,7 +89622,7 @@
     </row>
     <row r="615" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A615" t="s">
-        <v>3669</v>
+        <v>3668</v>
       </c>
       <c r="B615" s="1" t="s">
         <v>842</v>
@@ -89636,7 +89636,7 @@
     </row>
     <row r="616" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A616" t="s">
-        <v>3670</v>
+        <v>3669</v>
       </c>
       <c r="B616" s="1" t="s">
         <v>842</v>
@@ -89650,7 +89650,7 @@
     </row>
     <row r="617" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A617" t="s">
-        <v>3692</v>
+        <v>3691</v>
       </c>
       <c r="B617" s="1" t="s">
         <v>842</v>
@@ -90729,10 +90729,10 @@
         <v>1593</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>3564</v>
+        <v>3563</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>3509</v>
+        <v>3508</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="26" x14ac:dyDescent="0.35">
@@ -90743,10 +90743,10 @@
         <v>1593</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>3565</v>
+        <v>3564</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>3508</v>
+        <v>3507</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -90757,10 +90757,10 @@
         <v>1593</v>
       </c>
       <c r="C77" s="11" t="s">
+        <v>3505</v>
+      </c>
+      <c r="D77" s="11" t="s">
         <v>3506</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>3507</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -90771,10 +90771,10 @@
         <v>1593</v>
       </c>
       <c r="C78" s="11" t="s">
+        <v>3525</v>
+      </c>
+      <c r="D78" s="11" t="s">
         <v>3526</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>3527</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -90785,10 +90785,10 @@
         <v>1593</v>
       </c>
       <c r="C79" s="11" t="s">
+        <v>3560</v>
+      </c>
+      <c r="D79" s="11" t="s">
         <v>3561</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>3562</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -90799,10 +90799,10 @@
         <v>1593</v>
       </c>
       <c r="C80" s="11" t="s">
+        <v>3608</v>
+      </c>
+      <c r="D80" s="11" t="s">
         <v>3609</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>3610</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -90813,10 +90813,10 @@
         <v>1593</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -90827,10 +90827,10 @@
         <v>1593</v>
       </c>
       <c r="C82" s="11" t="s">
+        <v>3612</v>
+      </c>
+      <c r="D82" s="11" t="s">
         <v>3613</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>3614</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -90841,10 +90841,10 @@
         <v>1593</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>3616</v>
+        <v>3615</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -90855,38 +90855,38 @@
         <v>1593</v>
       </c>
       <c r="C84" s="11" t="s">
+        <v>3617</v>
+      </c>
+      <c r="D84" s="11" t="s">
         <v>3618</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>3619</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A85" s="12" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>3683</v>
+        <v>3682</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="26" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
-        <v>3657</v>
+        <v>3656</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>3688</v>
+        <v>3687</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="26" x14ac:dyDescent="0.35">
@@ -90894,13 +90894,13 @@
         <v>3411</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>3686</v>
+        <v>3685</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>3690</v>
+        <v>3689</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>3685</v>
+        <v>3684</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
@@ -90908,13 +90908,13 @@
         <v>2915</v>
       </c>
       <c r="B88" s="12" t="s">
+        <v>3685</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>3690</v>
+      </c>
+      <c r="D88" s="11" t="s">
         <v>3686</v>
-      </c>
-      <c r="C88" s="11" t="s">
-        <v>3691</v>
-      </c>
-      <c r="D88" s="11" t="s">
-        <v>3687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gundabad Orc Captaion shield cost
</commit_message>
<xml_diff>
--- a/src/mesbg_data.xlsx
+++ b/src/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE9BC8E-0468-468A-BEC9-2D7DF486CDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205045DF-524D-4FA4-BC57-AFAC260410C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -44024,9 +44024,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:G1643"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A376" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A389" sqref="A389:XFD389"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1482" sqref="D1482"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -75901,7 +75901,7 @@
         <v>309</v>
       </c>
       <c r="D1487" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1487" s="6">
         <v>0</v>
@@ -76533,7 +76533,7 @@
         <v>309</v>
       </c>
       <c r="D1518">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1518">
         <v>0</v>
@@ -77740,7 +77740,7 @@
         <v>309</v>
       </c>
       <c r="D1577" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F1577" s="6">
         <v>0</v>
@@ -79160,7 +79160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B3BDA4-C76D-4F2B-A5C7-6A022A2D593F}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A68" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
@@ -80397,7 +80397,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="312" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="299" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
         <v>957</v>
       </c>

</xml_diff>